<commit_message>
:books: docs: atualizar dicionário de dados com índices da pergunta 1
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionario_dados.xlsx
+++ b/dicionario_dados/dicionario_dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\codigos\projeto-bd2-satc\dicionario_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C325859-4D5A-4251-8DB5-2ECB699A43C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{739A3F6A-534A-4542-AF79-708F1224677F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="225">
   <si>
     <t>Tabela</t>
   </si>
@@ -815,6 +815,12 @@
     <t>pk_veiculos</t>
   </si>
   <si>
+    <t>idx_funcionarios_os_ordem_tempo_func</t>
+  </si>
+  <si>
+    <t>id_ordem_servico, tempo_trabalhado</t>
+  </si>
+  <si>
     <t>idx_historico_ordens_por_ordem_servico</t>
   </si>
   <si>
@@ -837,6 +843,12 @@
   </si>
   <si>
     <t>idx_ordens_data_saida</t>
+  </si>
+  <si>
+    <t>idx_ordens_status_data_entrada</t>
+  </si>
+  <si>
+    <t>status, data_entrada</t>
   </si>
 </sst>
 </file>
@@ -1282,50 +1294,146 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1333,111 +1441,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1752,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A588904-58D6-4340-A48F-92FCD18181A8}">
-  <dimension ref="A1:DU18"/>
+  <dimension ref="A1:DU19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DM1" workbookViewId="0">
-      <selection activeCell="DS14" sqref="DS14:DU14"/>
+    <sheetView tabSelected="1" topLeftCell="CB1" workbookViewId="0">
+      <selection activeCell="CD14" sqref="CD14:CK14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15"/>
@@ -1785,15 +1793,16 @@
     <col min="74" max="74" width="29.140625" customWidth="1"/>
     <col min="76" max="76" width="23.140625" customWidth="1"/>
     <col min="80" max="80" width="103.28515625" customWidth="1"/>
+    <col min="83" max="83" width="23.140625" customWidth="1"/>
     <col min="85" max="85" width="24" customWidth="1"/>
-    <col min="89" max="89" width="80.85546875" customWidth="1"/>
+    <col min="89" max="89" width="89" customWidth="1"/>
     <col min="92" max="92" width="24.42578125" customWidth="1"/>
     <col min="94" max="94" width="23.5703125" customWidth="1"/>
     <col min="98" max="98" width="82.5703125" customWidth="1"/>
     <col min="103" max="103" width="24.42578125" customWidth="1"/>
     <col min="107" max="107" width="89" customWidth="1"/>
     <col min="112" max="112" width="24.5703125" customWidth="1"/>
-    <col min="116" max="116" width="90.42578125" customWidth="1"/>
+    <col min="116" max="116" width="93.5703125" customWidth="1"/>
     <col min="119" max="119" width="23" customWidth="1"/>
     <col min="121" max="121" width="35" customWidth="1"/>
     <col min="125" max="125" width="102.5703125" customWidth="1"/>
@@ -1803,489 +1812,489 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
       <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
       <c r="S1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T1" s="31" t="s">
+      <c r="T1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="59"/>
       <c r="AB1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AC1" s="31" t="s">
+      <c r="AC1" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="59"/>
+      <c r="AF1" s="59"/>
+      <c r="AG1" s="59"/>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="59"/>
       <c r="AK1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AL1" s="31" t="s">
+      <c r="AL1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
+      <c r="AM1" s="59"/>
+      <c r="AN1" s="59"/>
+      <c r="AO1" s="59"/>
+      <c r="AP1" s="59"/>
+      <c r="AQ1" s="59"/>
+      <c r="AR1" s="59"/>
       <c r="AT1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AU1" s="31" t="s">
+      <c r="AU1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
+      <c r="AV1" s="59"/>
+      <c r="AW1" s="59"/>
+      <c r="AX1" s="59"/>
+      <c r="AY1" s="59"/>
+      <c r="AZ1" s="59"/>
+      <c r="BA1" s="59"/>
       <c r="BC1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="BD1" s="31" t="s">
+      <c r="BD1" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="31"/>
-      <c r="BH1" s="31"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
+      <c r="BE1" s="59"/>
+      <c r="BF1" s="59"/>
+      <c r="BG1" s="59"/>
+      <c r="BH1" s="59"/>
+      <c r="BI1" s="59"/>
+      <c r="BJ1" s="59"/>
       <c r="BL1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="BM1" s="31" t="s">
+      <c r="BM1" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="BN1" s="31"/>
-      <c r="BO1" s="31"/>
-      <c r="BP1" s="31"/>
-      <c r="BQ1" s="31"/>
-      <c r="BR1" s="31"/>
-      <c r="BS1" s="31"/>
+      <c r="BN1" s="59"/>
+      <c r="BO1" s="59"/>
+      <c r="BP1" s="59"/>
+      <c r="BQ1" s="59"/>
+      <c r="BR1" s="59"/>
+      <c r="BS1" s="59"/>
       <c r="BU1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="BV1" s="31" t="s">
+      <c r="BV1" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="BW1" s="31"/>
-      <c r="BX1" s="31"/>
-      <c r="BY1" s="31"/>
-      <c r="BZ1" s="31"/>
-      <c r="CA1" s="31"/>
-      <c r="CB1" s="31"/>
+      <c r="BW1" s="59"/>
+      <c r="BX1" s="59"/>
+      <c r="BY1" s="59"/>
+      <c r="BZ1" s="59"/>
+      <c r="CA1" s="59"/>
+      <c r="CB1" s="59"/>
       <c r="CD1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="CE1" s="31" t="s">
+      <c r="CE1" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="CF1" s="31"/>
-      <c r="CG1" s="31"/>
-      <c r="CH1" s="31"/>
-      <c r="CI1" s="31"/>
-      <c r="CJ1" s="31"/>
-      <c r="CK1" s="31"/>
+      <c r="CF1" s="59"/>
+      <c r="CG1" s="59"/>
+      <c r="CH1" s="59"/>
+      <c r="CI1" s="59"/>
+      <c r="CJ1" s="59"/>
+      <c r="CK1" s="59"/>
       <c r="CM1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="CN1" s="31" t="s">
+      <c r="CN1" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="CO1" s="31"/>
-      <c r="CP1" s="31"/>
-      <c r="CQ1" s="31"/>
-      <c r="CR1" s="31"/>
-      <c r="CS1" s="31"/>
-      <c r="CT1" s="31"/>
+      <c r="CO1" s="59"/>
+      <c r="CP1" s="59"/>
+      <c r="CQ1" s="59"/>
+      <c r="CR1" s="59"/>
+      <c r="CS1" s="59"/>
+      <c r="CT1" s="59"/>
       <c r="CV1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="CW1" s="31" t="s">
+      <c r="CW1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="CX1" s="31"/>
-      <c r="CY1" s="31"/>
-      <c r="CZ1" s="31"/>
-      <c r="DA1" s="31"/>
-      <c r="DB1" s="31"/>
-      <c r="DC1" s="31"/>
+      <c r="CX1" s="59"/>
+      <c r="CY1" s="59"/>
+      <c r="CZ1" s="59"/>
+      <c r="DA1" s="59"/>
+      <c r="DB1" s="59"/>
+      <c r="DC1" s="59"/>
       <c r="DE1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="DF1" s="31" t="s">
+      <c r="DF1" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="DG1" s="31"/>
-      <c r="DH1" s="31"/>
-      <c r="DI1" s="31"/>
-      <c r="DJ1" s="31"/>
-      <c r="DK1" s="31"/>
-      <c r="DL1" s="31"/>
+      <c r="DG1" s="59"/>
+      <c r="DH1" s="59"/>
+      <c r="DI1" s="59"/>
+      <c r="DJ1" s="59"/>
+      <c r="DK1" s="59"/>
+      <c r="DL1" s="59"/>
       <c r="DN1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="DO1" s="31" t="s">
+      <c r="DO1" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="DP1" s="31"/>
-      <c r="DQ1" s="31"/>
-      <c r="DR1" s="31"/>
-      <c r="DS1" s="31"/>
-      <c r="DT1" s="31"/>
-      <c r="DU1" s="31"/>
+      <c r="DP1" s="59"/>
+      <c r="DQ1" s="59"/>
+      <c r="DR1" s="59"/>
+      <c r="DS1" s="59"/>
+      <c r="DT1" s="59"/>
+      <c r="DU1" s="59"/>
     </row>
     <row r="2" spans="1:125" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
       <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
       <c r="S2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="31" t="s">
+      <c r="T2" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="59"/>
       <c r="AB2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AC2" s="31" t="s">
+      <c r="AC2" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="31"/>
-      <c r="AH2" s="31"/>
-      <c r="AI2" s="31"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="59"/>
+      <c r="AF2" s="59"/>
+      <c r="AG2" s="59"/>
+      <c r="AH2" s="59"/>
+      <c r="AI2" s="59"/>
       <c r="AK2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AL2" s="31" t="s">
+      <c r="AL2" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="AM2" s="31"/>
-      <c r="AN2" s="31"/>
-      <c r="AO2" s="31"/>
-      <c r="AP2" s="31"/>
-      <c r="AQ2" s="31"/>
-      <c r="AR2" s="31"/>
+      <c r="AM2" s="59"/>
+      <c r="AN2" s="59"/>
+      <c r="AO2" s="59"/>
+      <c r="AP2" s="59"/>
+      <c r="AQ2" s="59"/>
+      <c r="AR2" s="59"/>
       <c r="AT2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AU2" s="31" t="s">
+      <c r="AU2" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="AV2" s="31"/>
-      <c r="AW2" s="31"/>
-      <c r="AX2" s="31"/>
-      <c r="AY2" s="31"/>
-      <c r="AZ2" s="31"/>
-      <c r="BA2" s="31"/>
+      <c r="AV2" s="59"/>
+      <c r="AW2" s="59"/>
+      <c r="AX2" s="59"/>
+      <c r="AY2" s="59"/>
+      <c r="AZ2" s="59"/>
+      <c r="BA2" s="59"/>
       <c r="BC2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BD2" s="31" t="s">
+      <c r="BD2" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="BE2" s="31"/>
-      <c r="BF2" s="31"/>
-      <c r="BG2" s="31"/>
-      <c r="BH2" s="31"/>
-      <c r="BI2" s="31"/>
-      <c r="BJ2" s="31"/>
+      <c r="BE2" s="59"/>
+      <c r="BF2" s="59"/>
+      <c r="BG2" s="59"/>
+      <c r="BH2" s="59"/>
+      <c r="BI2" s="59"/>
+      <c r="BJ2" s="59"/>
       <c r="BL2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BM2" s="31" t="s">
+      <c r="BM2" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="BN2" s="31"/>
-      <c r="BO2" s="31"/>
-      <c r="BP2" s="31"/>
-      <c r="BQ2" s="31"/>
-      <c r="BR2" s="31"/>
-      <c r="BS2" s="31"/>
+      <c r="BN2" s="59"/>
+      <c r="BO2" s="59"/>
+      <c r="BP2" s="59"/>
+      <c r="BQ2" s="59"/>
+      <c r="BR2" s="59"/>
+      <c r="BS2" s="59"/>
       <c r="BU2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BV2" s="31" t="s">
+      <c r="BV2" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="BW2" s="31"/>
-      <c r="BX2" s="31"/>
-      <c r="BY2" s="31"/>
-      <c r="BZ2" s="31"/>
-      <c r="CA2" s="31"/>
-      <c r="CB2" s="31"/>
+      <c r="BW2" s="59"/>
+      <c r="BX2" s="59"/>
+      <c r="BY2" s="59"/>
+      <c r="BZ2" s="59"/>
+      <c r="CA2" s="59"/>
+      <c r="CB2" s="59"/>
       <c r="CD2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="CE2" s="54" t="s">
+      <c r="CE2" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="CF2" s="31"/>
-      <c r="CG2" s="31"/>
-      <c r="CH2" s="31"/>
-      <c r="CI2" s="31"/>
-      <c r="CJ2" s="31"/>
-      <c r="CK2" s="31"/>
+      <c r="CF2" s="59"/>
+      <c r="CG2" s="59"/>
+      <c r="CH2" s="59"/>
+      <c r="CI2" s="59"/>
+      <c r="CJ2" s="59"/>
+      <c r="CK2" s="59"/>
       <c r="CM2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="CN2" s="54" t="s">
+      <c r="CN2" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="CO2" s="31"/>
-      <c r="CP2" s="31"/>
-      <c r="CQ2" s="31"/>
-      <c r="CR2" s="31"/>
-      <c r="CS2" s="31"/>
-      <c r="CT2" s="31"/>
+      <c r="CO2" s="59"/>
+      <c r="CP2" s="59"/>
+      <c r="CQ2" s="59"/>
+      <c r="CR2" s="59"/>
+      <c r="CS2" s="59"/>
+      <c r="CT2" s="59"/>
       <c r="CV2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="CW2" s="31" t="s">
+      <c r="CW2" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="CX2" s="31"/>
-      <c r="CY2" s="31"/>
-      <c r="CZ2" s="31"/>
-      <c r="DA2" s="31"/>
-      <c r="DB2" s="31"/>
-      <c r="DC2" s="31"/>
+      <c r="CX2" s="59"/>
+      <c r="CY2" s="59"/>
+      <c r="CZ2" s="59"/>
+      <c r="DA2" s="59"/>
+      <c r="DB2" s="59"/>
+      <c r="DC2" s="59"/>
       <c r="DE2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="DF2" s="54" t="s">
+      <c r="DF2" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="DG2" s="31"/>
-      <c r="DH2" s="31"/>
-      <c r="DI2" s="31"/>
-      <c r="DJ2" s="31"/>
-      <c r="DK2" s="31"/>
-      <c r="DL2" s="31"/>
+      <c r="DG2" s="59"/>
+      <c r="DH2" s="59"/>
+      <c r="DI2" s="59"/>
+      <c r="DJ2" s="59"/>
+      <c r="DK2" s="59"/>
+      <c r="DL2" s="59"/>
       <c r="DN2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="DO2" s="31" t="s">
+      <c r="DO2" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="DP2" s="31"/>
-      <c r="DQ2" s="31"/>
-      <c r="DR2" s="31"/>
-      <c r="DS2" s="31"/>
-      <c r="DT2" s="31"/>
-      <c r="DU2" s="31"/>
+      <c r="DP2" s="59"/>
+      <c r="DQ2" s="59"/>
+      <c r="DR2" s="59"/>
+      <c r="DS2" s="59"/>
+      <c r="DT2" s="59"/>
+      <c r="DU2" s="59"/>
     </row>
     <row r="3" spans="1:125">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="J3" s="39" t="s">
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="J3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="S3" s="39" t="s">
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="S3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="39"/>
-      <c r="Y3" s="39"/>
-      <c r="Z3" s="39"/>
-      <c r="AB3" s="39" t="s">
+      <c r="T3" s="60"/>
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="60"/>
+      <c r="X3" s="60"/>
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="60"/>
+      <c r="AB3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="AC3" s="39"/>
-      <c r="AD3" s="39"/>
-      <c r="AE3" s="39"/>
-      <c r="AF3" s="39"/>
-      <c r="AG3" s="39"/>
-      <c r="AH3" s="39"/>
-      <c r="AI3" s="39"/>
-      <c r="AK3" s="39" t="s">
+      <c r="AC3" s="60"/>
+      <c r="AD3" s="60"/>
+      <c r="AE3" s="60"/>
+      <c r="AF3" s="60"/>
+      <c r="AG3" s="60"/>
+      <c r="AH3" s="60"/>
+      <c r="AI3" s="60"/>
+      <c r="AK3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="AL3" s="39"/>
-      <c r="AM3" s="39"/>
-      <c r="AN3" s="39"/>
-      <c r="AO3" s="39"/>
-      <c r="AP3" s="39"/>
-      <c r="AQ3" s="39"/>
-      <c r="AR3" s="39"/>
-      <c r="AT3" s="39" t="s">
+      <c r="AL3" s="60"/>
+      <c r="AM3" s="60"/>
+      <c r="AN3" s="60"/>
+      <c r="AO3" s="60"/>
+      <c r="AP3" s="60"/>
+      <c r="AQ3" s="60"/>
+      <c r="AR3" s="60"/>
+      <c r="AT3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="AU3" s="39"/>
-      <c r="AV3" s="39"/>
-      <c r="AW3" s="39"/>
-      <c r="AX3" s="39"/>
-      <c r="AY3" s="39"/>
-      <c r="AZ3" s="39"/>
-      <c r="BA3" s="39"/>
-      <c r="BC3" s="39" t="s">
+      <c r="AU3" s="60"/>
+      <c r="AV3" s="60"/>
+      <c r="AW3" s="60"/>
+      <c r="AX3" s="60"/>
+      <c r="AY3" s="60"/>
+      <c r="AZ3" s="60"/>
+      <c r="BA3" s="60"/>
+      <c r="BC3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="BD3" s="39"/>
-      <c r="BE3" s="39"/>
-      <c r="BF3" s="39"/>
-      <c r="BG3" s="39"/>
-      <c r="BH3" s="39"/>
-      <c r="BI3" s="39"/>
-      <c r="BJ3" s="39"/>
-      <c r="BL3" s="39" t="s">
+      <c r="BD3" s="60"/>
+      <c r="BE3" s="60"/>
+      <c r="BF3" s="60"/>
+      <c r="BG3" s="60"/>
+      <c r="BH3" s="60"/>
+      <c r="BI3" s="60"/>
+      <c r="BJ3" s="60"/>
+      <c r="BL3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="BM3" s="39"/>
-      <c r="BN3" s="39"/>
-      <c r="BO3" s="39"/>
-      <c r="BP3" s="39"/>
-      <c r="BQ3" s="39"/>
-      <c r="BR3" s="39"/>
-      <c r="BS3" s="39"/>
-      <c r="BU3" s="39" t="s">
+      <c r="BM3" s="60"/>
+      <c r="BN3" s="60"/>
+      <c r="BO3" s="60"/>
+      <c r="BP3" s="60"/>
+      <c r="BQ3" s="60"/>
+      <c r="BR3" s="60"/>
+      <c r="BS3" s="60"/>
+      <c r="BU3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="BV3" s="39"/>
-      <c r="BW3" s="39"/>
-      <c r="BX3" s="39"/>
-      <c r="BY3" s="39"/>
-      <c r="BZ3" s="39"/>
-      <c r="CA3" s="39"/>
-      <c r="CB3" s="39"/>
-      <c r="CD3" s="39" t="s">
+      <c r="BV3" s="60"/>
+      <c r="BW3" s="60"/>
+      <c r="BX3" s="60"/>
+      <c r="BY3" s="60"/>
+      <c r="BZ3" s="60"/>
+      <c r="CA3" s="60"/>
+      <c r="CB3" s="60"/>
+      <c r="CD3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="CE3" s="39"/>
-      <c r="CF3" s="39"/>
-      <c r="CG3" s="39"/>
-      <c r="CH3" s="39"/>
-      <c r="CI3" s="39"/>
-      <c r="CJ3" s="39"/>
-      <c r="CK3" s="39"/>
-      <c r="CM3" s="39" t="s">
+      <c r="CE3" s="60"/>
+      <c r="CF3" s="60"/>
+      <c r="CG3" s="60"/>
+      <c r="CH3" s="60"/>
+      <c r="CI3" s="60"/>
+      <c r="CJ3" s="60"/>
+      <c r="CK3" s="60"/>
+      <c r="CM3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="CN3" s="39"/>
-      <c r="CO3" s="39"/>
-      <c r="CP3" s="39"/>
-      <c r="CQ3" s="39"/>
-      <c r="CR3" s="39"/>
-      <c r="CS3" s="39"/>
-      <c r="CT3" s="39"/>
-      <c r="CV3" s="39" t="s">
+      <c r="CN3" s="60"/>
+      <c r="CO3" s="60"/>
+      <c r="CP3" s="60"/>
+      <c r="CQ3" s="60"/>
+      <c r="CR3" s="60"/>
+      <c r="CS3" s="60"/>
+      <c r="CT3" s="60"/>
+      <c r="CV3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="CW3" s="39"/>
-      <c r="CX3" s="39"/>
-      <c r="CY3" s="39"/>
-      <c r="CZ3" s="39"/>
-      <c r="DA3" s="39"/>
-      <c r="DB3" s="39"/>
-      <c r="DC3" s="39"/>
-      <c r="DE3" s="39" t="s">
+      <c r="CW3" s="60"/>
+      <c r="CX3" s="60"/>
+      <c r="CY3" s="60"/>
+      <c r="CZ3" s="60"/>
+      <c r="DA3" s="60"/>
+      <c r="DB3" s="60"/>
+      <c r="DC3" s="60"/>
+      <c r="DE3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="DF3" s="39"/>
-      <c r="DG3" s="39"/>
-      <c r="DH3" s="39"/>
-      <c r="DI3" s="39"/>
-      <c r="DJ3" s="39"/>
-      <c r="DK3" s="39"/>
-      <c r="DL3" s="39"/>
-      <c r="DN3" s="39" t="s">
+      <c r="DF3" s="60"/>
+      <c r="DG3" s="60"/>
+      <c r="DH3" s="60"/>
+      <c r="DI3" s="60"/>
+      <c r="DJ3" s="60"/>
+      <c r="DK3" s="60"/>
+      <c r="DL3" s="60"/>
+      <c r="DN3" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="DO3" s="39"/>
-      <c r="DP3" s="39"/>
-      <c r="DQ3" s="39"/>
-      <c r="DR3" s="39"/>
-      <c r="DS3" s="39"/>
-      <c r="DT3" s="39"/>
-      <c r="DU3" s="39"/>
+      <c r="DO3" s="60"/>
+      <c r="DP3" s="60"/>
+      <c r="DQ3" s="60"/>
+      <c r="DR3" s="60"/>
+      <c r="DS3" s="60"/>
+      <c r="DT3" s="60"/>
+      <c r="DU3" s="60"/>
     </row>
     <row r="4" spans="1:125">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="61"/>
       <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2304,10 +2313,10 @@
       <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="J4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="35"/>
+      <c r="K4" s="61"/>
       <c r="L4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2326,10 +2335,10 @@
       <c r="Q4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S4" s="35" t="s">
+      <c r="S4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="T4" s="35"/>
+      <c r="T4" s="61"/>
       <c r="U4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2348,10 +2357,10 @@
       <c r="Z4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="35" t="s">
+      <c r="AB4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="AC4" s="35"/>
+      <c r="AC4" s="61"/>
       <c r="AD4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2370,10 +2379,10 @@
       <c r="AI4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AK4" s="35" t="s">
+      <c r="AK4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="AL4" s="35"/>
+      <c r="AL4" s="61"/>
       <c r="AM4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2392,10 +2401,10 @@
       <c r="AR4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AT4" s="35" t="s">
+      <c r="AT4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="AU4" s="35"/>
+      <c r="AU4" s="61"/>
       <c r="AV4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2414,10 +2423,10 @@
       <c r="BA4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BC4" s="35" t="s">
+      <c r="BC4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="BD4" s="35"/>
+      <c r="BD4" s="61"/>
       <c r="BE4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2436,10 +2445,10 @@
       <c r="BJ4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BL4" s="35" t="s">
+      <c r="BL4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="BM4" s="35"/>
+      <c r="BM4" s="61"/>
       <c r="BN4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2458,10 +2467,10 @@
       <c r="BS4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BU4" s="35" t="s">
+      <c r="BU4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="BV4" s="35"/>
+      <c r="BV4" s="61"/>
       <c r="BW4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2480,10 +2489,10 @@
       <c r="CB4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="CD4" s="35" t="s">
+      <c r="CD4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="CE4" s="35"/>
+      <c r="CE4" s="61"/>
       <c r="CF4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2502,10 +2511,10 @@
       <c r="CK4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="CM4" s="35" t="s">
+      <c r="CM4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="CN4" s="35"/>
+      <c r="CN4" s="61"/>
       <c r="CO4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2524,10 +2533,10 @@
       <c r="CT4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="CV4" s="35" t="s">
+      <c r="CV4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="CW4" s="35"/>
+      <c r="CW4" s="61"/>
       <c r="CX4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2543,13 +2552,13 @@
       <c r="DB4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="DC4" s="64" t="s">
+      <c r="DC4" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="DE4" s="35" t="s">
+      <c r="DE4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="DF4" s="35"/>
+      <c r="DF4" s="61"/>
       <c r="DG4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2565,13 +2574,13 @@
       <c r="DK4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="DL4" s="64" t="s">
+      <c r="DL4" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="DN4" s="35" t="s">
+      <c r="DN4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="DO4" s="35"/>
+      <c r="DO4" s="61"/>
       <c r="DP4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2592,10 +2601,10 @@
       </c>
     </row>
     <row r="5" spans="1:125" ht="18.75" customHeight="1">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="31"/>
+      <c r="B5" s="59"/>
       <c r="C5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2612,10 +2621,10 @@
       <c r="H5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="J5" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="31"/>
+      <c r="K5" s="59"/>
       <c r="L5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2634,10 +2643,10 @@
       <c r="Q5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S5" s="31" t="s">
+      <c r="S5" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="T5" s="31"/>
+      <c r="T5" s="59"/>
       <c r="U5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2656,10 +2665,10 @@
       <c r="Z5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AB5" s="31" t="s">
+      <c r="AB5" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="AC5" s="31"/>
+      <c r="AC5" s="59"/>
       <c r="AD5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2678,10 +2687,10 @@
       <c r="AI5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AK5" s="31" t="s">
+      <c r="AK5" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="AL5" s="31"/>
+      <c r="AL5" s="59"/>
       <c r="AM5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2698,10 +2707,10 @@
       <c r="AR5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AT5" s="31" t="s">
+      <c r="AT5" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="AU5" s="31"/>
+      <c r="AU5" s="59"/>
       <c r="AV5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2718,10 +2727,10 @@
       <c r="BA5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="BC5" s="31" t="s">
+      <c r="BC5" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="BD5" s="31"/>
+      <c r="BD5" s="59"/>
       <c r="BE5" s="2" t="s">
         <v>47</v>
       </c>
@@ -2738,10 +2747,10 @@
       <c r="BJ5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="BL5" s="31" t="s">
+      <c r="BL5" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="BM5" s="31"/>
+      <c r="BM5" s="59"/>
       <c r="BN5" s="2" t="s">
         <v>50</v>
       </c>
@@ -2758,10 +2767,10 @@
       <c r="BS5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="BU5" s="31" t="s">
+      <c r="BU5" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="BV5" s="31"/>
+      <c r="BV5" s="59"/>
       <c r="BW5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2778,10 +2787,10 @@
       <c r="CB5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="CD5" s="31" t="s">
+      <c r="CD5" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="CE5" s="31"/>
+      <c r="CE5" s="59"/>
       <c r="CF5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2798,10 +2807,10 @@
       <c r="CK5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="CM5" s="31" t="s">
+      <c r="CM5" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="CN5" s="31"/>
+      <c r="CN5" s="59"/>
       <c r="CO5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2818,10 +2827,10 @@
       <c r="CT5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="CV5" s="31" t="s">
+      <c r="CV5" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="CW5" s="31"/>
+      <c r="CW5" s="59"/>
       <c r="CX5" s="2" t="s">
         <v>47</v>
       </c>
@@ -2834,14 +2843,14 @@
       <c r="DA5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="DB5" s="63"/>
-      <c r="DC5" s="62" t="s">
+      <c r="DB5" s="34"/>
+      <c r="DC5" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="DE5" s="31" t="s">
+      <c r="DE5" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="DF5" s="31"/>
+      <c r="DF5" s="59"/>
       <c r="DG5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2854,14 +2863,14 @@
       <c r="DJ5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="DK5" s="63"/>
-      <c r="DL5" s="62" t="s">
+      <c r="DK5" s="34"/>
+      <c r="DL5" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="DN5" s="31" t="s">
+      <c r="DN5" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="DO5" s="31"/>
+      <c r="DO5" s="59"/>
       <c r="DP5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2880,10 +2889,10 @@
       </c>
     </row>
     <row r="6" spans="1:125" ht="18" customHeight="1">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="31"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="2" t="s">
         <v>59</v>
       </c>
@@ -2898,10 +2907,10 @@
       <c r="H6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J6" s="31" t="s">
+      <c r="J6" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="K6" s="31"/>
+      <c r="K6" s="59"/>
       <c r="L6" s="2" t="s">
         <v>63</v>
       </c>
@@ -2916,10 +2925,10 @@
       <c r="Q6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S6" s="31" t="s">
+      <c r="S6" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="T6" s="31"/>
+      <c r="T6" s="59"/>
       <c r="U6" s="2" t="s">
         <v>67</v>
       </c>
@@ -2934,10 +2943,10 @@
       <c r="Z6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AB6" s="44" t="s">
+      <c r="AB6" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="AC6" s="44"/>
+      <c r="AC6" s="62"/>
       <c r="AD6" s="10" t="s">
         <v>71</v>
       </c>
@@ -2952,10 +2961,10 @@
       <c r="AI6" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="AK6" s="44" t="s">
+      <c r="AK6" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="AL6" s="44"/>
+      <c r="AL6" s="62"/>
       <c r="AM6" s="2" t="s">
         <v>38</v>
       </c>
@@ -2972,10 +2981,10 @@
       <c r="AR6" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="AT6" s="44" t="s">
+      <c r="AT6" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="AU6" s="44"/>
+      <c r="AU6" s="62"/>
       <c r="AV6" s="2" t="s">
         <v>74</v>
       </c>
@@ -2990,10 +2999,10 @@
       <c r="BA6" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="BC6" s="44" t="s">
+      <c r="BC6" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="BD6" s="44"/>
+      <c r="BD6" s="62"/>
       <c r="BE6" s="2" t="s">
         <v>59</v>
       </c>
@@ -3008,10 +3017,10 @@
       <c r="BJ6" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="BL6" s="31" t="s">
+      <c r="BL6" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="BM6" s="31"/>
+      <c r="BM6" s="59"/>
       <c r="BN6" s="2" t="s">
         <v>71</v>
       </c>
@@ -3026,10 +3035,10 @@
       <c r="BS6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="BU6" s="44" t="s">
+      <c r="BU6" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="BV6" s="44"/>
+      <c r="BV6" s="62"/>
       <c r="BW6" s="2" t="s">
         <v>38</v>
       </c>
@@ -3046,10 +3055,10 @@
       <c r="CB6" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="CD6" s="44" t="s">
+      <c r="CD6" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="CE6" s="44"/>
+      <c r="CE6" s="62"/>
       <c r="CF6" s="2" t="s">
         <v>38</v>
       </c>
@@ -3066,10 +3075,10 @@
       <c r="CK6" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="CM6" s="44" t="s">
+      <c r="CM6" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="CN6" s="44"/>
+      <c r="CN6" s="62"/>
       <c r="CO6" s="2" t="s">
         <v>38</v>
       </c>
@@ -3080,16 +3089,16 @@
         <v>40</v>
       </c>
       <c r="CR6" s="10"/>
-      <c r="CS6" s="60" t="s">
+      <c r="CS6" s="32" t="s">
         <v>41</v>
       </c>
       <c r="CT6" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="CV6" s="44" t="s">
+      <c r="CV6" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="CW6" s="44"/>
+      <c r="CW6" s="62"/>
       <c r="CX6" s="2" t="s">
         <v>59</v>
       </c>
@@ -3100,14 +3109,14 @@
         <v>40</v>
       </c>
       <c r="DA6" s="10"/>
-      <c r="DB6" s="60"/>
-      <c r="DC6" s="62" t="s">
+      <c r="DB6" s="32"/>
+      <c r="DC6" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="DE6" s="44" t="s">
+      <c r="DE6" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="DF6" s="44"/>
+      <c r="DF6" s="62"/>
       <c r="DG6" s="2" t="s">
         <v>38</v>
       </c>
@@ -3118,16 +3127,16 @@
         <v>40</v>
       </c>
       <c r="DJ6" s="10"/>
-      <c r="DK6" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="DL6" s="62" t="s">
+      <c r="DK6" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="DL6" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="DN6" s="44" t="s">
+      <c r="DN6" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="DO6" s="44"/>
+      <c r="DO6" s="62"/>
       <c r="DP6" s="2" t="s">
         <v>38</v>
       </c>
@@ -3146,10 +3155,10 @@
       </c>
     </row>
     <row r="7" spans="1:125" ht="17.25" customHeight="1">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="2" t="s">
         <v>88</v>
       </c>
@@ -3164,30 +3173,30 @@
       <c r="H7" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="34"/>
-      <c r="S7" s="32" t="s">
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="72"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="72"/>
+      <c r="Q7" s="45"/>
+      <c r="S7" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="T7" s="33"/>
-      <c r="U7" s="33"/>
-      <c r="V7" s="33"/>
-      <c r="W7" s="33"/>
-      <c r="X7" s="33"/>
-      <c r="Y7" s="33"/>
-      <c r="Z7" s="34"/>
-      <c r="AB7" s="42" t="s">
+      <c r="T7" s="72"/>
+      <c r="U7" s="72"/>
+      <c r="V7" s="72"/>
+      <c r="W7" s="72"/>
+      <c r="X7" s="72"/>
+      <c r="Y7" s="72"/>
+      <c r="Z7" s="45"/>
+      <c r="AB7" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="AC7" s="43"/>
+      <c r="AC7" s="57"/>
       <c r="AD7" s="9" t="s">
         <v>93</v>
       </c>
@@ -3202,10 +3211,10 @@
       <c r="AI7" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="AK7" s="42" t="s">
+      <c r="AK7" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="AL7" s="43"/>
+      <c r="AL7" s="57"/>
       <c r="AM7" s="9" t="s">
         <v>59</v>
       </c>
@@ -3220,10 +3229,10 @@
       <c r="AR7" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="AT7" s="42" t="s">
+      <c r="AT7" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="AU7" s="43"/>
+      <c r="AU7" s="57"/>
       <c r="AV7" s="9" t="s">
         <v>71</v>
       </c>
@@ -3238,10 +3247,10 @@
       <c r="BA7" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="BC7" s="42" t="s">
+      <c r="BC7" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="BD7" s="43"/>
+      <c r="BD7" s="57"/>
       <c r="BE7" s="9" t="s">
         <v>101</v>
       </c>
@@ -3256,20 +3265,20 @@
       <c r="BJ7" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="BL7" s="32" t="s">
+      <c r="BL7" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="BM7" s="33"/>
-      <c r="BN7" s="33"/>
-      <c r="BO7" s="33"/>
-      <c r="BP7" s="33"/>
-      <c r="BQ7" s="33"/>
-      <c r="BR7" s="33"/>
-      <c r="BS7" s="34"/>
-      <c r="BU7" s="42" t="s">
+      <c r="BM7" s="72"/>
+      <c r="BN7" s="72"/>
+      <c r="BO7" s="72"/>
+      <c r="BP7" s="72"/>
+      <c r="BQ7" s="72"/>
+      <c r="BR7" s="72"/>
+      <c r="BS7" s="45"/>
+      <c r="BU7" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="BV7" s="43"/>
+      <c r="BV7" s="57"/>
       <c r="BW7" s="9" t="s">
         <v>38</v>
       </c>
@@ -3286,10 +3295,10 @@
       <c r="CB7" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="CD7" s="42" t="s">
+      <c r="CD7" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="CE7" s="43"/>
+      <c r="CE7" s="57"/>
       <c r="CF7" s="9" t="s">
         <v>38</v>
       </c>
@@ -3306,10 +3315,10 @@
       <c r="CK7" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="CM7" s="42" t="s">
+      <c r="CM7" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="CN7" s="43"/>
+      <c r="CN7" s="57"/>
       <c r="CO7" s="9" t="s">
         <v>47</v>
       </c>
@@ -3326,28 +3335,28 @@
       <c r="CT7" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="CV7" s="42" t="s">
+      <c r="CV7" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="CW7" s="43"/>
+      <c r="CW7" s="57"/>
       <c r="CX7" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="CY7" s="57" t="s">
+      <c r="CY7" s="30" t="s">
         <v>102</v>
       </c>
       <c r="CZ7" s="9" t="s">
         <v>40</v>
       </c>
       <c r="DA7" s="9"/>
-      <c r="DB7" s="56"/>
+      <c r="DB7" s="29"/>
       <c r="DC7" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="DE7" s="42" t="s">
+      <c r="DE7" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="DF7" s="43"/>
+      <c r="DF7" s="57"/>
       <c r="DG7" s="2" t="s">
         <v>47</v>
       </c>
@@ -3358,16 +3367,16 @@
         <v>40</v>
       </c>
       <c r="DJ7" s="9"/>
-      <c r="DK7" s="56" t="s">
+      <c r="DK7" s="29" t="s">
         <v>41</v>
       </c>
       <c r="DL7" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="DN7" s="42" t="s">
+      <c r="DN7" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="DO7" s="43"/>
+      <c r="DO7" s="57"/>
       <c r="DP7" s="9" t="s">
         <v>38</v>
       </c>
@@ -3386,10 +3395,10 @@
       </c>
     </row>
     <row r="8" spans="1:125">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="2" t="s">
         <v>59</v>
       </c>
@@ -3404,10 +3413,10 @@
       <c r="H8" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="K8" s="35"/>
+      <c r="K8" s="61"/>
       <c r="L8" s="1" t="s">
         <v>116</v>
       </c>
@@ -3417,15 +3426,15 @@
       <c r="N8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="O8" s="35" t="s">
+      <c r="O8" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="35"/>
-      <c r="S8" s="35" t="s">
+      <c r="P8" s="61"/>
+      <c r="Q8" s="61"/>
+      <c r="S8" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="T8" s="35"/>
+      <c r="T8" s="61"/>
       <c r="U8" s="1" t="s">
         <v>116</v>
       </c>
@@ -3435,15 +3444,15 @@
       <c r="W8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="X8" s="35" t="s">
+      <c r="X8" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="Y8" s="35"/>
-      <c r="Z8" s="35"/>
-      <c r="AB8" s="42" t="s">
+      <c r="Y8" s="61"/>
+      <c r="Z8" s="61"/>
+      <c r="AB8" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="AC8" s="43"/>
+      <c r="AC8" s="57"/>
       <c r="AD8" s="9" t="s">
         <v>121</v>
       </c>
@@ -3458,10 +3467,10 @@
       <c r="AI8" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="AK8" s="42" t="s">
+      <c r="AK8" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="AL8" s="43"/>
+      <c r="AL8" s="57"/>
       <c r="AM8" s="9" t="s">
         <v>74</v>
       </c>
@@ -3476,10 +3485,10 @@
       <c r="AR8" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="AT8" s="42" t="s">
+      <c r="AT8" s="55" t="s">
         <v>126</v>
       </c>
-      <c r="AU8" s="43"/>
+      <c r="AU8" s="57"/>
       <c r="AV8" s="9" t="s">
         <v>71</v>
       </c>
@@ -3494,10 +3503,10 @@
       <c r="BA8" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="BC8" s="48" t="s">
+      <c r="BC8" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="BD8" s="49"/>
+      <c r="BD8" s="64"/>
       <c r="BE8" s="12" t="s">
         <v>129</v>
       </c>
@@ -3512,10 +3521,10 @@
       <c r="BJ8" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="BL8" s="35" t="s">
+      <c r="BL8" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="BM8" s="35"/>
+      <c r="BM8" s="61"/>
       <c r="BN8" s="1" t="s">
         <v>116</v>
       </c>
@@ -3525,15 +3534,15 @@
       <c r="BP8" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BQ8" s="35" t="s">
+      <c r="BQ8" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="BR8" s="35"/>
-      <c r="BS8" s="35"/>
-      <c r="BU8" s="42" t="s">
+      <c r="BR8" s="61"/>
+      <c r="BS8" s="61"/>
+      <c r="BU8" s="55" t="s">
         <v>132</v>
       </c>
-      <c r="BV8" s="43"/>
+      <c r="BV8" s="57"/>
       <c r="BW8" s="9" t="s">
         <v>93</v>
       </c>
@@ -3548,11 +3557,11 @@
       <c r="CB8" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="CD8" s="42" t="s">
+      <c r="CD8" s="55" t="s">
         <v>134</v>
       </c>
-      <c r="CE8" s="43"/>
-      <c r="CF8" s="55" t="s">
+      <c r="CE8" s="57"/>
+      <c r="CF8" s="28" t="s">
         <v>71</v>
       </c>
       <c r="CG8" s="13" t="s">
@@ -3566,11 +3575,11 @@
       <c r="CK8" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="CM8" s="48" t="s">
+      <c r="CM8" s="63" t="s">
         <v>136</v>
       </c>
-      <c r="CN8" s="49"/>
-      <c r="CO8" s="59" t="s">
+      <c r="CN8" s="64"/>
+      <c r="CO8" s="31" t="s">
         <v>129</v>
       </c>
       <c r="CP8" s="14" t="s">
@@ -3580,14 +3589,14 @@
         <v>40</v>
       </c>
       <c r="CR8" s="12"/>
-      <c r="CS8" s="56"/>
+      <c r="CS8" s="29"/>
       <c r="CT8" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="CV8" s="48" t="s">
+      <c r="CV8" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="CW8" s="49"/>
+      <c r="CW8" s="64"/>
       <c r="CX8" s="12" t="s">
         <v>38</v>
       </c>
@@ -3597,15 +3606,15 @@
       <c r="CZ8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="DA8" s="56"/>
+      <c r="DA8" s="29"/>
       <c r="DB8" s="9"/>
       <c r="DC8" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="DE8" s="48" t="s">
+      <c r="DE8" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="DF8" s="49"/>
+      <c r="DF8" s="64"/>
       <c r="DG8" s="12" t="s">
         <v>38</v>
       </c>
@@ -3615,15 +3624,15 @@
       <c r="DI8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="DJ8" s="56"/>
+      <c r="DJ8" s="29"/>
       <c r="DK8" s="9"/>
       <c r="DL8" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="DN8" s="42" t="s">
+      <c r="DN8" s="55" t="s">
         <v>142</v>
       </c>
-      <c r="DO8" s="43"/>
+      <c r="DO8" s="57"/>
       <c r="DP8" s="9" t="s">
         <v>143</v>
       </c>
@@ -3640,52 +3649,52 @@
       </c>
     </row>
     <row r="9" spans="1:125" ht="15.75" customHeight="1">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="J9" s="70" t="s">
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="J9" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="K9" s="71"/>
-      <c r="L9" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="M9" s="73"/>
-      <c r="N9" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="O9" s="70" t="s">
+      <c r="K9" s="43"/>
+      <c r="L9" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="71"/>
-      <c r="S9" s="70" t="s">
+      <c r="P9" s="50"/>
+      <c r="Q9" s="43"/>
+      <c r="S9" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="T9" s="71"/>
-      <c r="U9" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="V9" s="73"/>
-      <c r="W9" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="X9" s="70" t="s">
+      <c r="T9" s="43"/>
+      <c r="U9" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="V9" s="40"/>
+      <c r="W9" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="X9" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="Y9" s="74"/>
-      <c r="Z9" s="71"/>
-      <c r="AB9" s="42" t="s">
+      <c r="Y9" s="50"/>
+      <c r="Z9" s="43"/>
+      <c r="AB9" s="55" t="s">
         <v>148</v>
       </c>
-      <c r="AC9" s="43"/>
+      <c r="AC9" s="57"/>
       <c r="AD9" s="9" t="s">
         <v>129</v>
       </c>
@@ -3700,10 +3709,10 @@
       <c r="AI9" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="AK9" s="48" t="s">
+      <c r="AK9" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="AL9" s="49"/>
+      <c r="AL9" s="64"/>
       <c r="AM9" s="12" t="s">
         <v>71</v>
       </c>
@@ -3718,10 +3727,10 @@
       <c r="AR9" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="AT9" s="48" t="s">
+      <c r="AT9" s="63" t="s">
         <v>152</v>
       </c>
-      <c r="AU9" s="49"/>
+      <c r="AU9" s="64"/>
       <c r="AV9" s="12" t="s">
         <v>153</v>
       </c>
@@ -3739,17 +3748,17 @@
       <c r="BC9" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="BD9" s="52"/>
+      <c r="BD9" s="53"/>
       <c r="BE9" s="22"/>
       <c r="BF9" s="22"/>
       <c r="BG9" s="22"/>
       <c r="BH9" s="22"/>
       <c r="BI9" s="22"/>
       <c r="BJ9" s="22"/>
-      <c r="BL9" s="36" t="s">
+      <c r="BL9" s="69" t="s">
         <v>156</v>
       </c>
-      <c r="BM9" s="37"/>
+      <c r="BM9" s="70"/>
       <c r="BN9" s="4" t="s">
         <v>41</v>
       </c>
@@ -3757,15 +3766,15 @@
       <c r="BP9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="BQ9" s="36" t="s">
+      <c r="BQ9" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="BR9" s="38"/>
-      <c r="BS9" s="37"/>
-      <c r="BU9" s="48" t="s">
+      <c r="BR9" s="71"/>
+      <c r="BS9" s="70"/>
+      <c r="BU9" s="63" t="s">
         <v>157</v>
       </c>
-      <c r="BV9" s="49"/>
+      <c r="BV9" s="64"/>
       <c r="BW9" s="12" t="s">
         <v>93</v>
       </c>
@@ -3780,10 +3789,10 @@
       <c r="CB9" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="CD9" s="48" t="s">
+      <c r="CD9" s="63" t="s">
         <v>160</v>
       </c>
-      <c r="CE9" s="49"/>
+      <c r="CE9" s="64"/>
       <c r="CF9" s="12" t="s">
         <v>47</v>
       </c>
@@ -3794,24 +3803,24 @@
         <v>40</v>
       </c>
       <c r="CI9" s="12"/>
-      <c r="CJ9" s="56"/>
+      <c r="CJ9" s="29"/>
       <c r="CK9" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="CM9" s="58" t="s">
+      <c r="CM9" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="CN9" s="58"/>
-      <c r="CO9" s="58"/>
-      <c r="CP9" s="58"/>
-      <c r="CQ9" s="58"/>
-      <c r="CR9" s="58"/>
-      <c r="CS9" s="58"/>
-      <c r="CT9" s="61"/>
-      <c r="CV9" s="50" t="s">
+      <c r="CN9" s="54"/>
+      <c r="CO9" s="54"/>
+      <c r="CP9" s="54"/>
+      <c r="CQ9" s="54"/>
+      <c r="CR9" s="54"/>
+      <c r="CS9" s="54"/>
+      <c r="CT9" s="68"/>
+      <c r="CV9" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="CW9" s="50"/>
+      <c r="CW9" s="49"/>
       <c r="CX9" s="9" t="s">
         <v>129</v>
       </c>
@@ -3822,14 +3831,14 @@
         <v>40</v>
       </c>
       <c r="DA9" s="9"/>
-      <c r="DB9" s="65"/>
+      <c r="DB9" s="36"/>
       <c r="DC9" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="DE9" s="50" t="s">
+      <c r="DE9" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="DF9" s="50"/>
+      <c r="DF9" s="49"/>
       <c r="DG9" s="9" t="s">
         <v>129</v>
       </c>
@@ -3840,14 +3849,14 @@
         <v>40</v>
       </c>
       <c r="DJ9" s="9"/>
-      <c r="DK9" s="65"/>
+      <c r="DK9" s="36"/>
       <c r="DL9" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="DN9" s="48" t="s">
+      <c r="DN9" s="63" t="s">
         <v>166</v>
       </c>
-      <c r="DO9" s="49"/>
+      <c r="DO9" s="64"/>
       <c r="DP9" s="12" t="s">
         <v>93</v>
       </c>
@@ -3864,10 +3873,10 @@
       </c>
     </row>
     <row r="10" spans="1:125">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="35"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="1" t="s">
         <v>116</v>
       </c>
@@ -3877,15 +3886,15 @@
       <c r="E10" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="J10" s="50" t="s">
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="J10" s="49" t="s">
         <v>168</v>
       </c>
-      <c r="K10" s="50"/>
+      <c r="K10" s="49"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9" t="s">
         <v>41</v>
@@ -3893,15 +3902,15 @@
       <c r="N10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="O10" s="50" t="s">
+      <c r="O10" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="P10" s="50"/>
-      <c r="Q10" s="50"/>
-      <c r="S10" s="50" t="s">
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="S10" s="49" t="s">
         <v>169</v>
       </c>
-      <c r="T10" s="50"/>
+      <c r="T10" s="49"/>
       <c r="U10" s="9"/>
       <c r="V10" s="9" t="s">
         <v>41</v>
@@ -3909,25 +3918,25 @@
       <c r="W10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="X10" s="50" t="s">
+      <c r="X10" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="Y10" s="50"/>
-      <c r="Z10" s="50"/>
-      <c r="AB10" s="45" t="s">
+      <c r="Y10" s="49"/>
+      <c r="Z10" s="49"/>
+      <c r="AB10" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="AC10" s="46"/>
-      <c r="AD10" s="46"/>
-      <c r="AE10" s="46"/>
-      <c r="AF10" s="46"/>
-      <c r="AG10" s="46"/>
-      <c r="AH10" s="46"/>
-      <c r="AI10" s="47"/>
-      <c r="AK10" s="42" t="s">
+      <c r="AC10" s="73"/>
+      <c r="AD10" s="73"/>
+      <c r="AE10" s="73"/>
+      <c r="AF10" s="73"/>
+      <c r="AG10" s="73"/>
+      <c r="AH10" s="73"/>
+      <c r="AI10" s="67"/>
+      <c r="AK10" s="55" t="s">
         <v>170</v>
       </c>
-      <c r="AL10" s="43"/>
+      <c r="AL10" s="57"/>
       <c r="AM10" s="12" t="s">
         <v>71</v>
       </c>
@@ -3942,10 +3951,10 @@
       <c r="AR10" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="AT10" s="42" t="s">
+      <c r="AT10" s="55" t="s">
         <v>172</v>
       </c>
-      <c r="AU10" s="43"/>
+      <c r="AU10" s="57"/>
       <c r="AV10" s="12" t="s">
         <v>173</v>
       </c>
@@ -3960,10 +3969,10 @@
       <c r="BA10" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="BC10" s="66" t="s">
+      <c r="BC10" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="BD10" s="68"/>
+      <c r="BD10" s="48"/>
       <c r="BE10" s="24" t="s">
         <v>116</v>
       </c>
@@ -3973,15 +3982,15 @@
       <c r="BG10" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="BH10" s="66" t="s">
+      <c r="BH10" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="BI10" s="67"/>
-      <c r="BJ10" s="68"/>
-      <c r="BU10" s="48" t="s">
+      <c r="BI10" s="47"/>
+      <c r="BJ10" s="48"/>
+      <c r="BU10" s="63" t="s">
         <v>176</v>
       </c>
-      <c r="BV10" s="49"/>
+      <c r="BV10" s="64"/>
       <c r="BW10" s="12" t="s">
         <v>93</v>
       </c>
@@ -3996,14 +4005,14 @@
       <c r="CB10" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="CD10" s="50" t="s">
+      <c r="CD10" s="49" t="s">
         <v>178</v>
       </c>
-      <c r="CE10" s="50"/>
+      <c r="CE10" s="49"/>
       <c r="CF10" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="CG10" s="57" t="s">
+      <c r="CG10" s="30" t="s">
         <v>180</v>
       </c>
       <c r="CH10" s="9" t="s">
@@ -4014,10 +4023,10 @@
       <c r="CK10" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="CM10" s="45" t="s">
+      <c r="CM10" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="CN10" s="47"/>
+      <c r="CN10" s="67"/>
       <c r="CO10" s="24" t="s">
         <v>116</v>
       </c>
@@ -4035,31 +4044,31 @@
       <c r="CV10" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="CW10" s="69"/>
-      <c r="CX10" s="69"/>
-      <c r="CY10" s="69"/>
-      <c r="CZ10" s="69"/>
-      <c r="DA10" s="69"/>
-      <c r="DB10" s="69"/>
-      <c r="DC10" s="52"/>
+      <c r="CW10" s="52"/>
+      <c r="CX10" s="52"/>
+      <c r="CY10" s="52"/>
+      <c r="CZ10" s="52"/>
+      <c r="DA10" s="52"/>
+      <c r="DB10" s="52"/>
+      <c r="DC10" s="53"/>
       <c r="DE10" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="DF10" s="69"/>
-      <c r="DG10" s="69"/>
-      <c r="DH10" s="69"/>
-      <c r="DI10" s="69"/>
-      <c r="DJ10" s="69"/>
-      <c r="DK10" s="69"/>
-      <c r="DL10" s="52"/>
-      <c r="DN10" s="48" t="s">
+      <c r="DF10" s="52"/>
+      <c r="DG10" s="52"/>
+      <c r="DH10" s="52"/>
+      <c r="DI10" s="52"/>
+      <c r="DJ10" s="52"/>
+      <c r="DK10" s="52"/>
+      <c r="DL10" s="53"/>
+      <c r="DN10" s="63" t="s">
         <v>178</v>
       </c>
-      <c r="DO10" s="49"/>
+      <c r="DO10" s="64"/>
       <c r="DP10" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="DQ10" s="57" t="s">
+      <c r="DQ10" s="30" t="s">
         <v>102</v>
       </c>
       <c r="DR10" s="12" t="s">
@@ -4072,10 +4081,10 @@
       </c>
     </row>
     <row r="11" spans="1:125">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="75" t="s">
         <v>183</v>
       </c>
-      <c r="B11" s="41"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="8" t="s">
         <v>41</v>
       </c>
@@ -4083,15 +4092,15 @@
       <c r="E11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="41" t="s">
+      <c r="F11" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="AB11" s="35" t="s">
+      <c r="G11" s="75"/>
+      <c r="H11" s="75"/>
+      <c r="AB11" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="AC11" s="35"/>
+      <c r="AC11" s="61"/>
       <c r="AD11" s="1" t="s">
         <v>116</v>
       </c>
@@ -4101,15 +4110,15 @@
       <c r="AF11" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="AG11" s="35" t="s">
+      <c r="AG11" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="AH11" s="35"/>
-      <c r="AI11" s="35"/>
-      <c r="AK11" s="42" t="s">
+      <c r="AH11" s="61"/>
+      <c r="AI11" s="61"/>
+      <c r="AK11" s="55" t="s">
         <v>184</v>
       </c>
-      <c r="AL11" s="43"/>
+      <c r="AL11" s="57"/>
       <c r="AM11" s="12" t="s">
         <v>71</v>
       </c>
@@ -4124,10 +4133,10 @@
       <c r="AR11" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="AT11" s="48" t="s">
+      <c r="AT11" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="AU11" s="49"/>
+      <c r="AU11" s="64"/>
       <c r="AV11" s="12" t="s">
         <v>38</v>
       </c>
@@ -4142,10 +4151,10 @@
       <c r="BA11" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="BC11" s="36" t="s">
+      <c r="BC11" s="69" t="s">
         <v>189</v>
       </c>
-      <c r="BD11" s="37"/>
+      <c r="BD11" s="70"/>
       <c r="BE11" s="4" t="s">
         <v>41</v>
       </c>
@@ -4153,15 +4162,15 @@
       <c r="BG11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="BH11" s="36" t="s">
+      <c r="BH11" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="BI11" s="38"/>
-      <c r="BJ11" s="37"/>
-      <c r="BU11" s="50" t="s">
+      <c r="BI11" s="71"/>
+      <c r="BJ11" s="70"/>
+      <c r="BU11" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="BV11" s="50"/>
+      <c r="BV11" s="49"/>
       <c r="BW11" s="9" t="s">
         <v>59</v>
       </c>
@@ -4186,26 +4195,26 @@
       <c r="CI11" s="16"/>
       <c r="CJ11" s="16"/>
       <c r="CK11" s="17"/>
-      <c r="CM11" s="70" t="s">
+      <c r="CM11" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="CN11" s="71"/>
-      <c r="CO11" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="CP11" s="73"/>
-      <c r="CQ11" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="CR11" s="76" t="s">
+      <c r="CN11" s="43"/>
+      <c r="CO11" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="CP11" s="40"/>
+      <c r="CQ11" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="CR11" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="CS11" s="77"/>
-      <c r="CT11" s="78"/>
-      <c r="CV11" s="53" t="s">
+      <c r="CS11" s="41"/>
+      <c r="CT11" s="38"/>
+      <c r="CV11" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="CW11" s="53"/>
+      <c r="CW11" s="58"/>
       <c r="CX11" s="24" t="s">
         <v>116</v>
       </c>
@@ -4215,15 +4224,15 @@
       <c r="CZ11" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="DA11" s="53" t="s">
+      <c r="DA11" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="DB11" s="53"/>
-      <c r="DC11" s="53"/>
-      <c r="DE11" s="53" t="s">
+      <c r="DB11" s="58"/>
+      <c r="DC11" s="58"/>
+      <c r="DE11" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="DF11" s="53"/>
+      <c r="DF11" s="58"/>
       <c r="DG11" s="24" t="s">
         <v>116</v>
       </c>
@@ -4233,35 +4242,35 @@
       <c r="DI11" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="DJ11" s="53" t="s">
+      <c r="DJ11" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="DK11" s="53"/>
-      <c r="DL11" s="53"/>
-      <c r="DN11" s="66" t="s">
+      <c r="DK11" s="58"/>
+      <c r="DL11" s="58"/>
+      <c r="DN11" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="DO11" s="67"/>
-      <c r="DP11" s="67"/>
-      <c r="DQ11" s="67"/>
-      <c r="DR11" s="67"/>
-      <c r="DS11" s="67"/>
-      <c r="DT11" s="67"/>
-      <c r="DU11" s="68"/>
+      <c r="DO11" s="47"/>
+      <c r="DP11" s="47"/>
+      <c r="DQ11" s="47"/>
+      <c r="DR11" s="47"/>
+      <c r="DS11" s="47"/>
+      <c r="DT11" s="47"/>
+      <c r="DU11" s="48"/>
     </row>
     <row r="12" spans="1:125" ht="16.5" customHeight="1">
-      <c r="A12" s="40"/>
-      <c r="B12" s="40"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="AB12" s="36" t="s">
+      <c r="AB12" s="69" t="s">
         <v>193</v>
       </c>
-      <c r="AC12" s="37"/>
+      <c r="AC12" s="70"/>
       <c r="AD12" s="4" t="s">
         <v>41</v>
       </c>
@@ -4269,15 +4278,15 @@
       <c r="AF12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AG12" s="36" t="s">
+      <c r="AG12" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="AH12" s="38"/>
-      <c r="AI12" s="37"/>
-      <c r="AK12" s="42" t="s">
+      <c r="AH12" s="71"/>
+      <c r="AI12" s="70"/>
+      <c r="AK12" s="55" t="s">
         <v>194</v>
       </c>
-      <c r="AL12" s="43"/>
+      <c r="AL12" s="57"/>
       <c r="AM12" s="9" t="s">
         <v>195</v>
       </c>
@@ -4292,20 +4301,20 @@
       <c r="AR12" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="AT12" s="58" t="s">
+      <c r="AT12" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="AU12" s="58"/>
-      <c r="AV12" s="58"/>
-      <c r="AW12" s="58"/>
-      <c r="AX12" s="58"/>
-      <c r="AY12" s="58"/>
-      <c r="AZ12" s="58"/>
-      <c r="BA12" s="58"/>
-      <c r="BU12" s="48" t="s">
+      <c r="AU12" s="54"/>
+      <c r="AV12" s="54"/>
+      <c r="AW12" s="54"/>
+      <c r="AX12" s="54"/>
+      <c r="AY12" s="54"/>
+      <c r="AZ12" s="54"/>
+      <c r="BA12" s="54"/>
+      <c r="BU12" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="BV12" s="49"/>
+      <c r="BV12" s="64"/>
       <c r="BW12" s="12" t="s">
         <v>179</v>
       </c>
@@ -4320,10 +4329,10 @@
       <c r="CB12" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="CD12" s="32" t="s">
+      <c r="CD12" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="CE12" s="34"/>
+      <c r="CE12" s="45"/>
       <c r="CF12" s="1" t="s">
         <v>116</v>
       </c>
@@ -4333,29 +4342,29 @@
       <c r="CH12" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="CI12" s="32" t="s">
+      <c r="CI12" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="CJ12" s="33"/>
-      <c r="CK12" s="34"/>
-      <c r="CM12" s="50" t="s">
+      <c r="CJ12" s="72"/>
+      <c r="CK12" s="45"/>
+      <c r="CM12" s="49" t="s">
         <v>199</v>
       </c>
-      <c r="CN12" s="50"/>
+      <c r="CN12" s="49"/>
       <c r="CO12" s="9"/>
       <c r="CP12" s="9" t="s">
         <v>41</v>
       </c>
       <c r="CQ12" s="9"/>
-      <c r="CR12" s="50" t="s">
+      <c r="CR12" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="CS12" s="50"/>
-      <c r="CT12" s="50"/>
-      <c r="CV12" s="36" t="s">
+      <c r="CS12" s="49"/>
+      <c r="CT12" s="49"/>
+      <c r="CV12" s="69" t="s">
         <v>201</v>
       </c>
-      <c r="CW12" s="37"/>
+      <c r="CW12" s="70"/>
       <c r="CX12" s="4" t="s">
         <v>41</v>
       </c>
@@ -4363,31 +4372,31 @@
       <c r="CZ12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="DA12" s="36" t="s">
+      <c r="DA12" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="DB12" s="38"/>
-      <c r="DC12" s="37"/>
-      <c r="DE12" s="70" t="s">
+      <c r="DB12" s="71"/>
+      <c r="DC12" s="70"/>
+      <c r="DE12" s="42" t="s">
         <v>202</v>
       </c>
-      <c r="DF12" s="71"/>
-      <c r="DG12" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="DH12" s="73"/>
-      <c r="DI12" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="DJ12" s="70" t="s">
+      <c r="DF12" s="43"/>
+      <c r="DG12" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="DH12" s="40"/>
+      <c r="DI12" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="DJ12" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="DK12" s="74"/>
-      <c r="DL12" s="71"/>
-      <c r="DN12" s="32" t="s">
+      <c r="DK12" s="50"/>
+      <c r="DL12" s="43"/>
+      <c r="DN12" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="DO12" s="34"/>
+      <c r="DO12" s="45"/>
       <c r="DP12" s="1" t="s">
         <v>116</v>
       </c>
@@ -4397,25 +4406,25 @@
       <c r="DR12" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="DS12" s="28" t="s">
+      <c r="DS12" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="DT12" s="29"/>
-      <c r="DU12" s="30"/>
+      <c r="DT12" s="26"/>
+      <c r="DU12" s="27"/>
     </row>
     <row r="13" spans="1:125">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40"/>
+      <c r="A13" s="74"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="AK13" s="42" t="s">
+      <c r="AK13" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="AL13" s="43"/>
+      <c r="AL13" s="57"/>
       <c r="AM13" s="9" t="s">
         <v>74</v>
       </c>
@@ -4430,10 +4439,10 @@
       <c r="AR13" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="AT13" s="53" t="s">
+      <c r="AT13" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="AU13" s="53"/>
+      <c r="AU13" s="58"/>
       <c r="AV13" s="24" t="s">
         <v>116</v>
       </c>
@@ -4443,15 +4452,15 @@
       <c r="AX13" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="AY13" s="53" t="s">
+      <c r="AY13" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="AZ13" s="53"/>
-      <c r="BA13" s="53"/>
-      <c r="BU13" s="42" t="s">
+      <c r="AZ13" s="58"/>
+      <c r="BA13" s="58"/>
+      <c r="BU13" s="55" t="s">
         <v>205</v>
       </c>
-      <c r="BV13" s="43"/>
+      <c r="BV13" s="57"/>
       <c r="BW13" s="9" t="s">
         <v>50</v>
       </c>
@@ -4466,110 +4475,124 @@
       <c r="CB13" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="CD13" s="36" t="s">
+      <c r="CD13" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="CE13" s="37"/>
-      <c r="CF13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="CG13" s="3"/>
-      <c r="CH13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="CI13" s="25" t="s">
+      <c r="CE13" s="43"/>
+      <c r="CF13" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="CG13" s="40"/>
+      <c r="CH13" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="CI13" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="CJ13" s="26"/>
-      <c r="CK13" s="27"/>
-      <c r="DE13" s="50" t="s">
+      <c r="CJ13" s="41"/>
+      <c r="CK13" s="38"/>
+      <c r="DE13" s="49" t="s">
         <v>209</v>
       </c>
-      <c r="DF13" s="50"/>
+      <c r="DF13" s="49"/>
       <c r="DG13" s="9"/>
       <c r="DH13" s="9" t="s">
         <v>41</v>
       </c>
       <c r="DI13" s="9"/>
-      <c r="DJ13" s="50" t="s">
+      <c r="DJ13" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="DK13" s="50"/>
-      <c r="DL13" s="50"/>
-      <c r="DN13" s="70" t="s">
+      <c r="DK13" s="49"/>
+      <c r="DL13" s="49"/>
+      <c r="DN13" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="DO13" s="71"/>
-      <c r="DP13" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="DQ13" s="73"/>
-      <c r="DR13" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="DS13" s="70" t="s">
+      <c r="DO13" s="43"/>
+      <c r="DP13" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="DQ13" s="40"/>
+      <c r="DR13" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="DS13" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="DT13" s="74"/>
-      <c r="DU13" s="71"/>
+      <c r="DT13" s="50"/>
+      <c r="DU13" s="43"/>
     </row>
     <row r="14" spans="1:125" ht="15" customHeight="1">
-      <c r="AK14" s="45" t="s">
+      <c r="AK14" s="66" t="s">
         <v>91</v>
       </c>
-      <c r="AL14" s="46"/>
-      <c r="AM14" s="46"/>
-      <c r="AN14" s="46"/>
-      <c r="AO14" s="46"/>
-      <c r="AP14" s="46"/>
-      <c r="AQ14" s="46"/>
-      <c r="AR14" s="47"/>
-      <c r="AT14" s="70" t="s">
+      <c r="AL14" s="73"/>
+      <c r="AM14" s="73"/>
+      <c r="AN14" s="73"/>
+      <c r="AO14" s="73"/>
+      <c r="AP14" s="73"/>
+      <c r="AQ14" s="73"/>
+      <c r="AR14" s="67"/>
+      <c r="AT14" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="AU14" s="71"/>
-      <c r="AV14" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="AW14" s="73"/>
-      <c r="AX14" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="AY14" s="70" t="s">
+      <c r="AU14" s="43"/>
+      <c r="AV14" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW14" s="40"/>
+      <c r="AX14" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY14" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="AZ14" s="74"/>
-      <c r="BA14" s="71"/>
-      <c r="BU14" s="66" t="s">
+      <c r="AZ14" s="50"/>
+      <c r="BA14" s="43"/>
+      <c r="BU14" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="BV14" s="67"/>
-      <c r="BW14" s="67"/>
-      <c r="BX14" s="67"/>
-      <c r="BY14" s="67"/>
-      <c r="BZ14" s="67"/>
-      <c r="CA14" s="67"/>
-      <c r="CB14" s="68"/>
-      <c r="DN14" s="50" t="s">
+      <c r="BV14" s="47"/>
+      <c r="BW14" s="47"/>
+      <c r="BX14" s="47"/>
+      <c r="BY14" s="47"/>
+      <c r="BZ14" s="47"/>
+      <c r="CA14" s="47"/>
+      <c r="CB14" s="48"/>
+      <c r="CD14" s="49" t="s">
         <v>213</v>
       </c>
-      <c r="DO14" s="50"/>
+      <c r="CE14" s="49"/>
+      <c r="CF14" s="9"/>
+      <c r="CG14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="CH14" s="9"/>
+      <c r="CI14" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="CJ14" s="49"/>
+      <c r="CK14" s="49"/>
+      <c r="DN14" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="DO14" s="49"/>
       <c r="DP14" s="9"/>
       <c r="DQ14" s="9" t="s">
         <v>41</v>
       </c>
       <c r="DR14" s="9"/>
-      <c r="DS14" s="50" t="s">
-        <v>214</v>
-      </c>
-      <c r="DT14" s="50"/>
-      <c r="DU14" s="50"/>
+      <c r="DS14" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="DT14" s="49"/>
+      <c r="DU14" s="49"/>
     </row>
     <row r="15" spans="1:125" ht="15" customHeight="1">
-      <c r="AK15" s="35" t="s">
+      <c r="AK15" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="AL15" s="35"/>
+      <c r="AL15" s="61"/>
       <c r="AM15" s="1" t="s">
         <v>116</v>
       </c>
@@ -4579,15 +4602,15 @@
       <c r="AO15" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="AP15" s="35" t="s">
+      <c r="AP15" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="AQ15" s="35"/>
-      <c r="AR15" s="35"/>
-      <c r="AT15" s="50" t="s">
-        <v>215</v>
-      </c>
-      <c r="AU15" s="50"/>
+      <c r="AQ15" s="61"/>
+      <c r="AR15" s="61"/>
+      <c r="AT15" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="AU15" s="49"/>
       <c r="AV15" s="9"/>
       <c r="AW15" s="9" t="s">
         <v>41</v>
@@ -4595,15 +4618,15 @@
       <c r="AX15" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AY15" s="42" t="s">
+      <c r="AY15" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="AZ15" s="75"/>
-      <c r="BA15" s="43"/>
-      <c r="BU15" s="32" t="s">
+      <c r="AZ15" s="56"/>
+      <c r="BA15" s="57"/>
+      <c r="BU15" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="BV15" s="34"/>
+      <c r="BV15" s="45"/>
       <c r="BW15" s="1" t="s">
         <v>116</v>
       </c>
@@ -4613,17 +4636,25 @@
       <c r="BY15" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="BZ15" s="28" t="s">
+      <c r="BZ15" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="CA15" s="29"/>
-      <c r="CB15" s="30"/>
+      <c r="CA15" s="26"/>
+      <c r="CB15" s="27"/>
+      <c r="CD15" s="77"/>
+      <c r="CE15" s="77"/>
+      <c r="CF15" s="78"/>
+      <c r="CG15" s="78"/>
+      <c r="CH15" s="78"/>
+      <c r="CI15" s="77"/>
+      <c r="CJ15" s="77"/>
+      <c r="CK15" s="77"/>
     </row>
     <row r="16" spans="1:125" ht="15.75" customHeight="1">
-      <c r="AK16" s="36" t="s">
-        <v>216</v>
-      </c>
-      <c r="AL16" s="37"/>
+      <c r="AK16" s="69" t="s">
+        <v>218</v>
+      </c>
+      <c r="AL16" s="70"/>
       <c r="AM16" s="4" t="s">
         <v>41</v>
       </c>
@@ -4631,207 +4662,122 @@
       <c r="AO16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AP16" s="36" t="s">
+      <c r="AP16" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="AQ16" s="38"/>
-      <c r="AR16" s="37"/>
-      <c r="BU16" s="70" t="s">
-        <v>217</v>
-      </c>
-      <c r="BV16" s="71"/>
-      <c r="BW16" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="BX16" s="73"/>
-      <c r="BY16" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="BZ16" s="76" t="s">
+      <c r="AQ16" s="71"/>
+      <c r="AR16" s="70"/>
+      <c r="BU16" s="42" t="s">
+        <v>219</v>
+      </c>
+      <c r="BV16" s="43"/>
+      <c r="BW16" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="BX16" s="40"/>
+      <c r="BY16" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="BZ16" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="CA16" s="77"/>
-      <c r="CB16" s="78"/>
+      <c r="CA16" s="41"/>
+      <c r="CB16" s="38"/>
     </row>
     <row r="17" spans="73:80">
-      <c r="BU17" s="50" t="s">
-        <v>218</v>
-      </c>
-      <c r="BV17" s="50"/>
+      <c r="BU17" s="49" t="s">
+        <v>220</v>
+      </c>
+      <c r="BV17" s="49"/>
       <c r="BW17" s="9"/>
       <c r="BX17" s="9" t="s">
         <v>41</v>
       </c>
       <c r="BY17" s="9"/>
-      <c r="BZ17" s="50" t="s">
-        <v>219</v>
-      </c>
-      <c r="CA17" s="50"/>
-      <c r="CB17" s="50"/>
+      <c r="BZ17" s="49" t="s">
+        <v>221</v>
+      </c>
+      <c r="CA17" s="49"/>
+      <c r="CB17" s="49"/>
     </row>
     <row r="18" spans="73:80">
-      <c r="BU18" s="50" t="s">
-        <v>220</v>
-      </c>
-      <c r="BV18" s="50"/>
-      <c r="BW18" s="9"/>
-      <c r="BX18" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="BY18" s="9"/>
-      <c r="BZ18" s="50" t="s">
+      <c r="BU18" s="76" t="s">
+        <v>222</v>
+      </c>
+      <c r="BV18" s="76"/>
+      <c r="BW18" s="12"/>
+      <c r="BX18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="BY18" s="12"/>
+      <c r="BZ18" s="76" t="s">
         <v>157</v>
       </c>
-      <c r="CA18" s="50"/>
-      <c r="CB18" s="50"/>
+      <c r="CA18" s="76"/>
+      <c r="CB18" s="76"/>
+    </row>
+    <row r="19" spans="73:80">
+      <c r="BU19" s="49" t="s">
+        <v>223</v>
+      </c>
+      <c r="BV19" s="49"/>
+      <c r="BW19" s="9"/>
+      <c r="BX19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="BY19" s="9"/>
+      <c r="BZ19" s="49" t="s">
+        <v>224</v>
+      </c>
+      <c r="CA19" s="49"/>
+      <c r="CB19" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="207">
-    <mergeCell ref="BU16:BV16"/>
-    <mergeCell ref="BU15:BV15"/>
-    <mergeCell ref="BU14:CB14"/>
-    <mergeCell ref="BU17:BV17"/>
-    <mergeCell ref="BU18:BV18"/>
-    <mergeCell ref="BZ17:CB17"/>
-    <mergeCell ref="BZ18:CB18"/>
-    <mergeCell ref="DE13:DF13"/>
-    <mergeCell ref="DJ13:DL13"/>
-    <mergeCell ref="DN14:DO14"/>
-    <mergeCell ref="DS13:DU13"/>
-    <mergeCell ref="DN13:DO13"/>
-    <mergeCell ref="DE10:DL10"/>
-    <mergeCell ref="CV10:DC10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="AT15:AU15"/>
-    <mergeCell ref="AT12:BA12"/>
-    <mergeCell ref="AY15:BA15"/>
-    <mergeCell ref="BH10:BJ10"/>
-    <mergeCell ref="DN11:DU11"/>
-    <mergeCell ref="DS14:DU14"/>
-    <mergeCell ref="DE11:DF11"/>
-    <mergeCell ref="DJ11:DL11"/>
-    <mergeCell ref="DE12:DF12"/>
-    <mergeCell ref="DJ12:DL12"/>
-    <mergeCell ref="DO1:DU1"/>
-    <mergeCell ref="DO2:DU2"/>
-    <mergeCell ref="DN3:DU3"/>
-    <mergeCell ref="DN4:DO4"/>
-    <mergeCell ref="DN5:DO5"/>
-    <mergeCell ref="DN6:DO6"/>
-    <mergeCell ref="DN7:DO7"/>
-    <mergeCell ref="DN8:DO8"/>
-    <mergeCell ref="DN9:DO9"/>
-    <mergeCell ref="DN10:DO10"/>
-    <mergeCell ref="DN12:DO12"/>
-    <mergeCell ref="DF1:DL1"/>
-    <mergeCell ref="DF2:DL2"/>
-    <mergeCell ref="DE3:DL3"/>
-    <mergeCell ref="DE4:DF4"/>
-    <mergeCell ref="DE5:DF5"/>
-    <mergeCell ref="DE6:DF6"/>
-    <mergeCell ref="DE7:DF7"/>
-    <mergeCell ref="DE8:DF8"/>
-    <mergeCell ref="DE9:DF9"/>
-    <mergeCell ref="CM10:CN10"/>
-    <mergeCell ref="CM12:CN12"/>
-    <mergeCell ref="CR12:CT12"/>
-    <mergeCell ref="CM11:CN11"/>
-    <mergeCell ref="CM9:CT9"/>
-    <mergeCell ref="CW1:DC1"/>
-    <mergeCell ref="CW2:DC2"/>
-    <mergeCell ref="CV3:DC3"/>
-    <mergeCell ref="CV4:CW4"/>
-    <mergeCell ref="CV5:CW5"/>
-    <mergeCell ref="CV6:CW6"/>
-    <mergeCell ref="CV7:CW7"/>
-    <mergeCell ref="CV8:CW8"/>
-    <mergeCell ref="CV9:CW9"/>
-    <mergeCell ref="CV11:CW11"/>
-    <mergeCell ref="DA11:DC11"/>
-    <mergeCell ref="CV12:CW12"/>
-    <mergeCell ref="DA12:DC12"/>
-    <mergeCell ref="CN1:CT1"/>
-    <mergeCell ref="CN2:CT2"/>
-    <mergeCell ref="CM3:CT3"/>
-    <mergeCell ref="CM4:CN4"/>
-    <mergeCell ref="CM5:CN5"/>
-    <mergeCell ref="CM6:CN6"/>
-    <mergeCell ref="CM7:CN7"/>
-    <mergeCell ref="CM8:CN8"/>
-    <mergeCell ref="BU10:BV10"/>
-    <mergeCell ref="BU11:BV11"/>
-    <mergeCell ref="BU13:BV13"/>
-    <mergeCell ref="BU12:BV12"/>
-    <mergeCell ref="CE1:CK1"/>
-    <mergeCell ref="CE2:CK2"/>
-    <mergeCell ref="CD3:CK3"/>
-    <mergeCell ref="CD4:CE4"/>
-    <mergeCell ref="CD5:CE5"/>
-    <mergeCell ref="CD6:CE6"/>
-    <mergeCell ref="CD7:CE7"/>
-    <mergeCell ref="CD8:CE8"/>
-    <mergeCell ref="CD9:CE9"/>
-    <mergeCell ref="CD10:CE10"/>
-    <mergeCell ref="CD12:CE12"/>
-    <mergeCell ref="CI12:CK12"/>
-    <mergeCell ref="CD13:CE13"/>
-    <mergeCell ref="BV1:CB1"/>
-    <mergeCell ref="BV2:CB2"/>
-    <mergeCell ref="BU3:CB3"/>
-    <mergeCell ref="BU4:BV4"/>
-    <mergeCell ref="BU5:BV5"/>
-    <mergeCell ref="BU6:BV6"/>
-    <mergeCell ref="BU7:BV7"/>
-    <mergeCell ref="BU8:BV8"/>
-    <mergeCell ref="BU9:BV9"/>
-    <mergeCell ref="BH11:BJ11"/>
-    <mergeCell ref="AT14:AU14"/>
-    <mergeCell ref="AY14:BA14"/>
-    <mergeCell ref="BD1:BJ1"/>
-    <mergeCell ref="BD2:BJ2"/>
-    <mergeCell ref="BC3:BJ3"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="BC7:BD7"/>
-    <mergeCell ref="BC8:BD8"/>
-    <mergeCell ref="BC9:BD9"/>
-    <mergeCell ref="BC10:BD10"/>
-    <mergeCell ref="BC11:BD11"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="AU2:BA2"/>
-    <mergeCell ref="AT3:BA3"/>
-    <mergeCell ref="AT4:AU4"/>
-    <mergeCell ref="AT5:AU5"/>
-    <mergeCell ref="AT11:AU11"/>
-    <mergeCell ref="AT13:AU13"/>
-    <mergeCell ref="AY13:BA13"/>
-    <mergeCell ref="AT6:AU6"/>
-    <mergeCell ref="AT7:AU7"/>
-    <mergeCell ref="AT8:AU8"/>
-    <mergeCell ref="AT9:AU9"/>
-    <mergeCell ref="AT10:AU10"/>
-    <mergeCell ref="AK14:AR14"/>
-    <mergeCell ref="AK15:AL15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AK16:AL16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AK10:AL10"/>
-    <mergeCell ref="AK11:AL11"/>
-    <mergeCell ref="AK12:AL12"/>
-    <mergeCell ref="AK13:AL13"/>
-    <mergeCell ref="AL1:AR1"/>
-    <mergeCell ref="AL2:AR2"/>
-    <mergeCell ref="AK3:AR3"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="AK7:AL7"/>
-    <mergeCell ref="AK8:AL8"/>
-    <mergeCell ref="AK9:AL9"/>
+  <mergeCells count="213">
+    <mergeCell ref="BZ19:CB19"/>
+    <mergeCell ref="BU19:BV19"/>
+    <mergeCell ref="CD14:CE14"/>
+    <mergeCell ref="CI14:CK14"/>
+    <mergeCell ref="CD15:CE15"/>
+    <mergeCell ref="CI15:CK15"/>
+    <mergeCell ref="BL6:BM6"/>
+    <mergeCell ref="BL7:BS7"/>
+    <mergeCell ref="BL8:BM8"/>
+    <mergeCell ref="BQ8:BS8"/>
+    <mergeCell ref="BL9:BM9"/>
+    <mergeCell ref="BQ9:BS9"/>
+    <mergeCell ref="BM1:BS1"/>
+    <mergeCell ref="BM2:BS2"/>
+    <mergeCell ref="BL3:BS3"/>
+    <mergeCell ref="BL4:BM4"/>
+    <mergeCell ref="BL5:BM5"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="X8:Z8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="O9:Q9"/>
+    <mergeCell ref="J7:Q7"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="K2:Q2"/>
+    <mergeCell ref="J3:Q3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="S9:T9"/>
     <mergeCell ref="X9:Z9"/>
     <mergeCell ref="AC1:AI1"/>
@@ -4856,44 +4802,151 @@
     <mergeCell ref="S6:T6"/>
     <mergeCell ref="S7:Z7"/>
     <mergeCell ref="S8:T8"/>
-    <mergeCell ref="X8:Z8"/>
-    <mergeCell ref="O8:Q8"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="J7:Q7"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="K1:Q1"/>
-    <mergeCell ref="K2:Q2"/>
-    <mergeCell ref="J3:Q3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="BL6:BM6"/>
-    <mergeCell ref="BL7:BS7"/>
-    <mergeCell ref="BL8:BM8"/>
-    <mergeCell ref="BQ8:BS8"/>
-    <mergeCell ref="BL9:BM9"/>
-    <mergeCell ref="BQ9:BS9"/>
-    <mergeCell ref="BM1:BS1"/>
-    <mergeCell ref="BM2:BS2"/>
-    <mergeCell ref="BL3:BS3"/>
-    <mergeCell ref="BL4:BM4"/>
-    <mergeCell ref="BL5:BM5"/>
+    <mergeCell ref="AK15:AL15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AK16:AL16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AK10:AL10"/>
+    <mergeCell ref="AK11:AL11"/>
+    <mergeCell ref="AK12:AL12"/>
+    <mergeCell ref="AK13:AL13"/>
+    <mergeCell ref="AL1:AR1"/>
+    <mergeCell ref="AL2:AR2"/>
+    <mergeCell ref="AK3:AR3"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="AK7:AL7"/>
+    <mergeCell ref="AK8:AL8"/>
+    <mergeCell ref="AK9:AL9"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="AU2:BA2"/>
+    <mergeCell ref="AT3:BA3"/>
+    <mergeCell ref="AT4:AU4"/>
+    <mergeCell ref="AT5:AU5"/>
+    <mergeCell ref="AT11:AU11"/>
+    <mergeCell ref="AT13:AU13"/>
+    <mergeCell ref="AY13:BA13"/>
+    <mergeCell ref="AT6:AU6"/>
+    <mergeCell ref="AT7:AU7"/>
+    <mergeCell ref="AT8:AU8"/>
+    <mergeCell ref="AT9:AU9"/>
+    <mergeCell ref="AT10:AU10"/>
+    <mergeCell ref="BD1:BJ1"/>
+    <mergeCell ref="BD2:BJ2"/>
+    <mergeCell ref="BC3:BJ3"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="BC7:BD7"/>
+    <mergeCell ref="BC8:BD8"/>
+    <mergeCell ref="BC9:BD9"/>
+    <mergeCell ref="BV1:CB1"/>
+    <mergeCell ref="BV2:CB2"/>
+    <mergeCell ref="BU3:CB3"/>
+    <mergeCell ref="BU4:BV4"/>
+    <mergeCell ref="BU5:BV5"/>
+    <mergeCell ref="BU6:BV6"/>
+    <mergeCell ref="BU7:BV7"/>
+    <mergeCell ref="BU8:BV8"/>
+    <mergeCell ref="BU9:BV9"/>
+    <mergeCell ref="CE1:CK1"/>
+    <mergeCell ref="CE2:CK2"/>
+    <mergeCell ref="CD3:CK3"/>
+    <mergeCell ref="CD4:CE4"/>
+    <mergeCell ref="CD5:CE5"/>
+    <mergeCell ref="CD6:CE6"/>
+    <mergeCell ref="CD7:CE7"/>
+    <mergeCell ref="CD8:CE8"/>
+    <mergeCell ref="CD9:CE9"/>
+    <mergeCell ref="CM9:CT9"/>
+    <mergeCell ref="CW1:DC1"/>
+    <mergeCell ref="CW2:DC2"/>
+    <mergeCell ref="CV3:DC3"/>
+    <mergeCell ref="CV4:CW4"/>
+    <mergeCell ref="CV5:CW5"/>
+    <mergeCell ref="CV6:CW6"/>
+    <mergeCell ref="CV7:CW7"/>
+    <mergeCell ref="CV8:CW8"/>
+    <mergeCell ref="CV9:CW9"/>
+    <mergeCell ref="CN1:CT1"/>
+    <mergeCell ref="CN2:CT2"/>
+    <mergeCell ref="CM3:CT3"/>
+    <mergeCell ref="CM4:CN4"/>
+    <mergeCell ref="CM5:CN5"/>
+    <mergeCell ref="CM6:CN6"/>
+    <mergeCell ref="CM7:CN7"/>
+    <mergeCell ref="CM8:CN8"/>
+    <mergeCell ref="DF1:DL1"/>
+    <mergeCell ref="DF2:DL2"/>
+    <mergeCell ref="DE3:DL3"/>
+    <mergeCell ref="DE4:DF4"/>
+    <mergeCell ref="DE5:DF5"/>
+    <mergeCell ref="DE6:DF6"/>
+    <mergeCell ref="DE7:DF7"/>
+    <mergeCell ref="DE8:DF8"/>
+    <mergeCell ref="DE9:DF9"/>
+    <mergeCell ref="DO1:DU1"/>
+    <mergeCell ref="DO2:DU2"/>
+    <mergeCell ref="DN3:DU3"/>
+    <mergeCell ref="DN4:DO4"/>
+    <mergeCell ref="DN5:DO5"/>
+    <mergeCell ref="DN6:DO6"/>
+    <mergeCell ref="DN7:DO7"/>
+    <mergeCell ref="DN8:DO8"/>
+    <mergeCell ref="DN9:DO9"/>
+    <mergeCell ref="AT15:AU15"/>
+    <mergeCell ref="AT12:BA12"/>
+    <mergeCell ref="AY15:BA15"/>
+    <mergeCell ref="BH10:BJ10"/>
+    <mergeCell ref="DN11:DU11"/>
+    <mergeCell ref="DS14:DU14"/>
+    <mergeCell ref="DE11:DF11"/>
+    <mergeCell ref="DJ11:DL11"/>
+    <mergeCell ref="DE12:DF12"/>
+    <mergeCell ref="DJ12:DL12"/>
+    <mergeCell ref="DN10:DO10"/>
+    <mergeCell ref="DN12:DO12"/>
+    <mergeCell ref="CM10:CN10"/>
+    <mergeCell ref="CM12:CN12"/>
+    <mergeCell ref="CR12:CT12"/>
+    <mergeCell ref="CM11:CN11"/>
+    <mergeCell ref="CV11:CW11"/>
+    <mergeCell ref="DA11:DC11"/>
+    <mergeCell ref="CV12:CW12"/>
+    <mergeCell ref="DA12:DC12"/>
+    <mergeCell ref="BU10:BV10"/>
+    <mergeCell ref="BU11:BV11"/>
+    <mergeCell ref="BU13:BV13"/>
+    <mergeCell ref="BU12:BV12"/>
+    <mergeCell ref="DN14:DO14"/>
+    <mergeCell ref="DS13:DU13"/>
+    <mergeCell ref="DN13:DO13"/>
+    <mergeCell ref="DE10:DL10"/>
+    <mergeCell ref="CV10:DC10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="CD10:CE10"/>
+    <mergeCell ref="CD12:CE12"/>
+    <mergeCell ref="CI12:CK12"/>
+    <mergeCell ref="CD13:CE13"/>
+    <mergeCell ref="BH11:BJ11"/>
+    <mergeCell ref="AT14:AU14"/>
+    <mergeCell ref="AY14:BA14"/>
+    <mergeCell ref="BC10:BD10"/>
+    <mergeCell ref="BC11:BD11"/>
+    <mergeCell ref="AK14:AR14"/>
+    <mergeCell ref="BU16:BV16"/>
+    <mergeCell ref="BU15:BV15"/>
+    <mergeCell ref="BU14:CB14"/>
+    <mergeCell ref="BU17:BV17"/>
+    <mergeCell ref="BU18:BV18"/>
+    <mergeCell ref="BZ17:CB17"/>
+    <mergeCell ref="BZ18:CB18"/>
+    <mergeCell ref="DE13:DF13"/>
+    <mergeCell ref="DJ13:DL13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
:pencil: style: corrigir erros ortográficos no dicionário de dados
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionario_dados.xlsx
+++ b/dicionario_dados/dicionario_dados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29016"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\codigos\projeto-bd2-satc\dicionario_dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\satc.edu.br\dados\Usuarios\lucas.flores\Meus Documentos\Projetos\abp-bd2\dicionario_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{739A3F6A-534A-4542-AF79-708F1224677F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD86C037-08FB-460E-9FF0-A3F1F8D2BCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="226">
   <si>
     <t>Tabela</t>
   </si>
@@ -332,9 +332,6 @@
     <t>1 – 255</t>
   </si>
   <si>
-    <t>Código de identificação da odem de serviço</t>
-  </si>
-  <si>
     <t>Identificador único do registro na tabela</t>
   </si>
   <si>
@@ -344,9 +341,6 @@
     <t>Código de identificação da peça em estoque</t>
   </si>
   <si>
-    <t>Código de identificação da peça na ordem de servico</t>
-  </si>
-  <si>
     <t>Identificador único do registro no histórico</t>
   </si>
   <si>
@@ -416,9 +410,6 @@
     <t>id_veiculo</t>
   </si>
   <si>
-    <t>Chave estrangeira que referencia o veículo associado à ordem</t>
-  </si>
-  <si>
     <t>id_ordem_de_servico</t>
   </si>
   <si>
@@ -431,12 +422,6 @@
     <t>id_ordem_servico</t>
   </si>
   <si>
-    <t xml:space="preserve">Chave estrangeira que referencia a ordem de serviço </t>
-  </si>
-  <si>
-    <t>Chave estrangeira que referencia a pessoa (funcionário) responsável pela alteração</t>
-  </si>
-  <si>
     <t>telefone</t>
   </si>
   <si>
@@ -491,30 +476,18 @@
     <t>id_cliente</t>
   </si>
   <si>
-    <t>Chave estrangeira que referencia o cliente que solicitou o serviço.</t>
-  </si>
-  <si>
     <t>id_funcionario</t>
   </si>
   <si>
-    <t xml:space="preserve">Chave estrangeira que referencia o funcionário </t>
-  </si>
-  <si>
     <t>id_servico</t>
   </si>
   <si>
-    <t>Chave estrangeira que referencia o serviço executado</t>
-  </si>
-  <si>
     <t>Campo para detalhar características técnicas da peça e observações relevantes para uso ou reposição.</t>
   </si>
   <si>
     <t>id_peca</t>
   </si>
   <si>
-    <t>Chave estrangeira que referencia a peça utilizada</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -740,18 +713,12 @@
     <t>1 - 2.147.483.647</t>
   </si>
   <si>
-    <t>Distância que o veículo percorreu desde sua fabriacação</t>
-  </si>
-  <si>
     <t>pk_servicos</t>
   </si>
   <si>
     <t>titulo</t>
   </si>
   <si>
-    <t>Frase que, de forma resumida, descreve e nomeia  a ordem de serviço</t>
-  </si>
-  <si>
     <t>pk_itens_servicos_os</t>
   </si>
   <si>
@@ -767,9 +734,6 @@
     <t>1 - 2</t>
   </si>
   <si>
-    <t>Sigla da unidade da federação qie identifica o estado no qual o endereço está localizado</t>
-  </si>
-  <si>
     <t>Campo destinado a descrever detalhadamente os serviços a serem prestados ou qualquer outra informação relevante</t>
   </si>
   <si>
@@ -797,9 +761,6 @@
     <t>1 - 255</t>
   </si>
   <si>
-    <t>Define o progresso no qual a ordem de serviso se encontra</t>
-  </si>
-  <si>
     <t>pk_funcionarios_os</t>
   </si>
   <si>
@@ -849,13 +810,55 @@
   </si>
   <si>
     <t>status, data_entrada</t>
+  </si>
+  <si>
+    <t>Sigla da unidade da federação que identifica o estado no qual o endereço está localizado</t>
+  </si>
+  <si>
+    <t>Distância que o veículo percorreu desde sua fabricação</t>
+  </si>
+  <si>
+    <t>Código de identificação da ordem de serviço</t>
+  </si>
+  <si>
+    <t>Chave estrangeira que referência o veículo associado à ordem</t>
+  </si>
+  <si>
+    <t>Chave estrangeira que referência o cliente que solicitou o serviço.</t>
+  </si>
+  <si>
+    <t>Define o progresso no qual a ordem de serviço se encontra</t>
+  </si>
+  <si>
+    <t>Frase que, de forma resumida, descreve e nomeia a ordem de serviço</t>
+  </si>
+  <si>
+    <t>Chave estrangeira que refêrencia a ordem de serviço</t>
+  </si>
+  <si>
+    <t>Chave estrangeira que refêrencia o serviço executado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chave estrangeira que indica o funcionário </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chave estrangeira que referência a ordem de serviço </t>
+  </si>
+  <si>
+    <t>Chave estrangeira que referência a peça utilizada</t>
+  </si>
+  <si>
+    <t>Código de identificação da peça na ordem de serviço</t>
+  </si>
+  <si>
+    <t>Chave estrangeira que referência a pessoa (funcionário) responsável pela alteração</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1238,7 +1241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1294,15 +1297,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1339,17 +1333,97 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1360,92 +1434,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1464,9 +1470,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1504,7 +1510,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1610,7 +1616,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1752,7 +1758,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1762,11 +1768,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A588904-58D6-4340-A48F-92FCD18181A8}">
   <dimension ref="A1:DU19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CB1" workbookViewId="0">
-      <selection activeCell="CD14" sqref="CD14:CK14"/>
+    <sheetView tabSelected="1" topLeftCell="DQ1" workbookViewId="0">
+      <selection activeCell="DU7" sqref="DU7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="3.85546875" customWidth="1"/>
@@ -1792,7 +1798,7 @@
     <col min="67" max="67" width="23.7109375" customWidth="1"/>
     <col min="74" max="74" width="29.140625" customWidth="1"/>
     <col min="76" max="76" width="23.140625" customWidth="1"/>
-    <col min="80" max="80" width="103.28515625" customWidth="1"/>
+    <col min="80" max="80" width="105" customWidth="1"/>
     <col min="83" max="83" width="23.140625" customWidth="1"/>
     <col min="85" max="85" width="24" customWidth="1"/>
     <col min="89" max="89" width="89" customWidth="1"/>
@@ -1808,493 +1814,493 @@
     <col min="125" max="125" width="102.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:125" ht="20.25" customHeight="1">
+    <row r="1" spans="1:125" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
       <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
       <c r="S1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T1" s="59" t="s">
+      <c r="T1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="U1" s="59"/>
-      <c r="V1" s="59"/>
-      <c r="W1" s="59"/>
-      <c r="X1" s="59"/>
-      <c r="Y1" s="59"/>
-      <c r="Z1" s="59"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
       <c r="AB1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AC1" s="59" t="s">
+      <c r="AC1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="59"/>
-      <c r="AE1" s="59"/>
-      <c r="AF1" s="59"/>
-      <c r="AG1" s="59"/>
-      <c r="AH1" s="59"/>
-      <c r="AI1" s="59"/>
+      <c r="AD1" s="42"/>
+      <c r="AE1" s="42"/>
+      <c r="AF1" s="42"/>
+      <c r="AG1" s="42"/>
+      <c r="AH1" s="42"/>
+      <c r="AI1" s="42"/>
       <c r="AK1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AL1" s="59" t="s">
+      <c r="AL1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="AM1" s="59"/>
-      <c r="AN1" s="59"/>
-      <c r="AO1" s="59"/>
-      <c r="AP1" s="59"/>
-      <c r="AQ1" s="59"/>
-      <c r="AR1" s="59"/>
+      <c r="AM1" s="42"/>
+      <c r="AN1" s="42"/>
+      <c r="AO1" s="42"/>
+      <c r="AP1" s="42"/>
+      <c r="AQ1" s="42"/>
+      <c r="AR1" s="42"/>
       <c r="AT1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AU1" s="59" t="s">
+      <c r="AU1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="59"/>
-      <c r="AW1" s="59"/>
-      <c r="AX1" s="59"/>
-      <c r="AY1" s="59"/>
-      <c r="AZ1" s="59"/>
-      <c r="BA1" s="59"/>
+      <c r="AV1" s="42"/>
+      <c r="AW1" s="42"/>
+      <c r="AX1" s="42"/>
+      <c r="AY1" s="42"/>
+      <c r="AZ1" s="42"/>
+      <c r="BA1" s="42"/>
       <c r="BC1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="BD1" s="59" t="s">
+      <c r="BD1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="BE1" s="59"/>
-      <c r="BF1" s="59"/>
-      <c r="BG1" s="59"/>
-      <c r="BH1" s="59"/>
-      <c r="BI1" s="59"/>
-      <c r="BJ1" s="59"/>
+      <c r="BE1" s="42"/>
+      <c r="BF1" s="42"/>
+      <c r="BG1" s="42"/>
+      <c r="BH1" s="42"/>
+      <c r="BI1" s="42"/>
+      <c r="BJ1" s="42"/>
       <c r="BL1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="BM1" s="59" t="s">
+      <c r="BM1" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="BN1" s="59"/>
-      <c r="BO1" s="59"/>
-      <c r="BP1" s="59"/>
-      <c r="BQ1" s="59"/>
-      <c r="BR1" s="59"/>
-      <c r="BS1" s="59"/>
+      <c r="BN1" s="42"/>
+      <c r="BO1" s="42"/>
+      <c r="BP1" s="42"/>
+      <c r="BQ1" s="42"/>
+      <c r="BR1" s="42"/>
+      <c r="BS1" s="42"/>
       <c r="BU1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="BV1" s="59" t="s">
+      <c r="BV1" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="BW1" s="59"/>
-      <c r="BX1" s="59"/>
-      <c r="BY1" s="59"/>
-      <c r="BZ1" s="59"/>
-      <c r="CA1" s="59"/>
-      <c r="CB1" s="59"/>
+      <c r="BW1" s="42"/>
+      <c r="BX1" s="42"/>
+      <c r="BY1" s="42"/>
+      <c r="BZ1" s="42"/>
+      <c r="CA1" s="42"/>
+      <c r="CB1" s="42"/>
       <c r="CD1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="CE1" s="59" t="s">
+      <c r="CE1" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="CF1" s="59"/>
-      <c r="CG1" s="59"/>
-      <c r="CH1" s="59"/>
-      <c r="CI1" s="59"/>
-      <c r="CJ1" s="59"/>
-      <c r="CK1" s="59"/>
+      <c r="CF1" s="42"/>
+      <c r="CG1" s="42"/>
+      <c r="CH1" s="42"/>
+      <c r="CI1" s="42"/>
+      <c r="CJ1" s="42"/>
+      <c r="CK1" s="42"/>
       <c r="CM1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="CN1" s="59" t="s">
+      <c r="CN1" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="CO1" s="59"/>
-      <c r="CP1" s="59"/>
-      <c r="CQ1" s="59"/>
-      <c r="CR1" s="59"/>
-      <c r="CS1" s="59"/>
-      <c r="CT1" s="59"/>
+      <c r="CO1" s="42"/>
+      <c r="CP1" s="42"/>
+      <c r="CQ1" s="42"/>
+      <c r="CR1" s="42"/>
+      <c r="CS1" s="42"/>
+      <c r="CT1" s="42"/>
       <c r="CV1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="CW1" s="59" t="s">
+      <c r="CW1" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="CX1" s="59"/>
-      <c r="CY1" s="59"/>
-      <c r="CZ1" s="59"/>
-      <c r="DA1" s="59"/>
-      <c r="DB1" s="59"/>
-      <c r="DC1" s="59"/>
+      <c r="CX1" s="42"/>
+      <c r="CY1" s="42"/>
+      <c r="CZ1" s="42"/>
+      <c r="DA1" s="42"/>
+      <c r="DB1" s="42"/>
+      <c r="DC1" s="42"/>
       <c r="DE1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="DF1" s="59" t="s">
+      <c r="DF1" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="DG1" s="59"/>
-      <c r="DH1" s="59"/>
-      <c r="DI1" s="59"/>
-      <c r="DJ1" s="59"/>
-      <c r="DK1" s="59"/>
-      <c r="DL1" s="59"/>
+      <c r="DG1" s="42"/>
+      <c r="DH1" s="42"/>
+      <c r="DI1" s="42"/>
+      <c r="DJ1" s="42"/>
+      <c r="DK1" s="42"/>
+      <c r="DL1" s="42"/>
       <c r="DN1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="DO1" s="59" t="s">
+      <c r="DO1" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="DP1" s="59"/>
-      <c r="DQ1" s="59"/>
-      <c r="DR1" s="59"/>
-      <c r="DS1" s="59"/>
-      <c r="DT1" s="59"/>
-      <c r="DU1" s="59"/>
+      <c r="DP1" s="42"/>
+      <c r="DQ1" s="42"/>
+      <c r="DR1" s="42"/>
+      <c r="DS1" s="42"/>
+      <c r="DT1" s="42"/>
+      <c r="DU1" s="42"/>
     </row>
-    <row r="2" spans="1:125" ht="15" customHeight="1">
+    <row r="2" spans="1:125" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
       <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="59" t="s">
+      <c r="K2" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
       <c r="S2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="59" t="s">
+      <c r="T2" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="59"/>
-      <c r="Z2" s="59"/>
+      <c r="U2" s="42"/>
+      <c r="V2" s="42"/>
+      <c r="W2" s="42"/>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="42"/>
+      <c r="Z2" s="42"/>
       <c r="AB2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AC2" s="59" t="s">
+      <c r="AC2" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="AD2" s="59"/>
-      <c r="AE2" s="59"/>
-      <c r="AF2" s="59"/>
-      <c r="AG2" s="59"/>
-      <c r="AH2" s="59"/>
-      <c r="AI2" s="59"/>
+      <c r="AD2" s="42"/>
+      <c r="AE2" s="42"/>
+      <c r="AF2" s="42"/>
+      <c r="AG2" s="42"/>
+      <c r="AH2" s="42"/>
+      <c r="AI2" s="42"/>
       <c r="AK2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AL2" s="59" t="s">
+      <c r="AL2" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="AM2" s="59"/>
-      <c r="AN2" s="59"/>
-      <c r="AO2" s="59"/>
-      <c r="AP2" s="59"/>
-      <c r="AQ2" s="59"/>
-      <c r="AR2" s="59"/>
+      <c r="AM2" s="42"/>
+      <c r="AN2" s="42"/>
+      <c r="AO2" s="42"/>
+      <c r="AP2" s="42"/>
+      <c r="AQ2" s="42"/>
+      <c r="AR2" s="42"/>
       <c r="AT2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AU2" s="59" t="s">
+      <c r="AU2" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="AV2" s="59"/>
-      <c r="AW2" s="59"/>
-      <c r="AX2" s="59"/>
-      <c r="AY2" s="59"/>
-      <c r="AZ2" s="59"/>
-      <c r="BA2" s="59"/>
+      <c r="AV2" s="42"/>
+      <c r="AW2" s="42"/>
+      <c r="AX2" s="42"/>
+      <c r="AY2" s="42"/>
+      <c r="AZ2" s="42"/>
+      <c r="BA2" s="42"/>
       <c r="BC2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BD2" s="59" t="s">
+      <c r="BD2" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="BE2" s="59"/>
-      <c r="BF2" s="59"/>
-      <c r="BG2" s="59"/>
-      <c r="BH2" s="59"/>
-      <c r="BI2" s="59"/>
-      <c r="BJ2" s="59"/>
+      <c r="BE2" s="42"/>
+      <c r="BF2" s="42"/>
+      <c r="BG2" s="42"/>
+      <c r="BH2" s="42"/>
+      <c r="BI2" s="42"/>
+      <c r="BJ2" s="42"/>
       <c r="BL2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BM2" s="59" t="s">
+      <c r="BM2" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="BN2" s="59"/>
-      <c r="BO2" s="59"/>
-      <c r="BP2" s="59"/>
-      <c r="BQ2" s="59"/>
-      <c r="BR2" s="59"/>
-      <c r="BS2" s="59"/>
+      <c r="BN2" s="42"/>
+      <c r="BO2" s="42"/>
+      <c r="BP2" s="42"/>
+      <c r="BQ2" s="42"/>
+      <c r="BR2" s="42"/>
+      <c r="BS2" s="42"/>
       <c r="BU2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BV2" s="59" t="s">
+      <c r="BV2" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="BW2" s="59"/>
-      <c r="BX2" s="59"/>
-      <c r="BY2" s="59"/>
-      <c r="BZ2" s="59"/>
-      <c r="CA2" s="59"/>
-      <c r="CB2" s="59"/>
+      <c r="BW2" s="42"/>
+      <c r="BX2" s="42"/>
+      <c r="BY2" s="42"/>
+      <c r="BZ2" s="42"/>
+      <c r="CA2" s="42"/>
+      <c r="CB2" s="42"/>
       <c r="CD2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="CE2" s="65" t="s">
+      <c r="CE2" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="CF2" s="59"/>
-      <c r="CG2" s="59"/>
-      <c r="CH2" s="59"/>
-      <c r="CI2" s="59"/>
-      <c r="CJ2" s="59"/>
-      <c r="CK2" s="59"/>
+      <c r="CF2" s="42"/>
+      <c r="CG2" s="42"/>
+      <c r="CH2" s="42"/>
+      <c r="CI2" s="42"/>
+      <c r="CJ2" s="42"/>
+      <c r="CK2" s="42"/>
       <c r="CM2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="CN2" s="65" t="s">
+      <c r="CN2" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="CO2" s="59"/>
-      <c r="CP2" s="59"/>
-      <c r="CQ2" s="59"/>
-      <c r="CR2" s="59"/>
-      <c r="CS2" s="59"/>
-      <c r="CT2" s="59"/>
+      <c r="CO2" s="42"/>
+      <c r="CP2" s="42"/>
+      <c r="CQ2" s="42"/>
+      <c r="CR2" s="42"/>
+      <c r="CS2" s="42"/>
+      <c r="CT2" s="42"/>
       <c r="CV2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="CW2" s="59" t="s">
+      <c r="CW2" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="CX2" s="59"/>
-      <c r="CY2" s="59"/>
-      <c r="CZ2" s="59"/>
-      <c r="DA2" s="59"/>
-      <c r="DB2" s="59"/>
-      <c r="DC2" s="59"/>
+      <c r="CX2" s="42"/>
+      <c r="CY2" s="42"/>
+      <c r="CZ2" s="42"/>
+      <c r="DA2" s="42"/>
+      <c r="DB2" s="42"/>
+      <c r="DC2" s="42"/>
       <c r="DE2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="DF2" s="65" t="s">
+      <c r="DF2" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="DG2" s="59"/>
-      <c r="DH2" s="59"/>
-      <c r="DI2" s="59"/>
-      <c r="DJ2" s="59"/>
-      <c r="DK2" s="59"/>
-      <c r="DL2" s="59"/>
+      <c r="DG2" s="42"/>
+      <c r="DH2" s="42"/>
+      <c r="DI2" s="42"/>
+      <c r="DJ2" s="42"/>
+      <c r="DK2" s="42"/>
+      <c r="DL2" s="42"/>
       <c r="DN2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="DO2" s="59" t="s">
+      <c r="DO2" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="DP2" s="59"/>
-      <c r="DQ2" s="59"/>
-      <c r="DR2" s="59"/>
-      <c r="DS2" s="59"/>
-      <c r="DT2" s="59"/>
-      <c r="DU2" s="59"/>
+      <c r="DP2" s="42"/>
+      <c r="DQ2" s="42"/>
+      <c r="DR2" s="42"/>
+      <c r="DS2" s="42"/>
+      <c r="DT2" s="42"/>
+      <c r="DU2" s="42"/>
     </row>
-    <row r="3" spans="1:125">
-      <c r="A3" s="60" t="s">
+    <row r="3" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="J3" s="60" t="s">
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="J3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
-      <c r="S3" s="60" t="s">
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="S3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="T3" s="60"/>
-      <c r="U3" s="60"/>
-      <c r="V3" s="60"/>
-      <c r="W3" s="60"/>
-      <c r="X3" s="60"/>
-      <c r="Y3" s="60"/>
-      <c r="Z3" s="60"/>
-      <c r="AB3" s="60" t="s">
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
+      <c r="Y3" s="50"/>
+      <c r="Z3" s="50"/>
+      <c r="AB3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="AC3" s="60"/>
-      <c r="AD3" s="60"/>
-      <c r="AE3" s="60"/>
-      <c r="AF3" s="60"/>
-      <c r="AG3" s="60"/>
-      <c r="AH3" s="60"/>
-      <c r="AI3" s="60"/>
-      <c r="AK3" s="60" t="s">
+      <c r="AC3" s="50"/>
+      <c r="AD3" s="50"/>
+      <c r="AE3" s="50"/>
+      <c r="AF3" s="50"/>
+      <c r="AG3" s="50"/>
+      <c r="AH3" s="50"/>
+      <c r="AI3" s="50"/>
+      <c r="AK3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="AL3" s="60"/>
-      <c r="AM3" s="60"/>
-      <c r="AN3" s="60"/>
-      <c r="AO3" s="60"/>
-      <c r="AP3" s="60"/>
-      <c r="AQ3" s="60"/>
-      <c r="AR3" s="60"/>
-      <c r="AT3" s="60" t="s">
+      <c r="AL3" s="50"/>
+      <c r="AM3" s="50"/>
+      <c r="AN3" s="50"/>
+      <c r="AO3" s="50"/>
+      <c r="AP3" s="50"/>
+      <c r="AQ3" s="50"/>
+      <c r="AR3" s="50"/>
+      <c r="AT3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="AU3" s="60"/>
-      <c r="AV3" s="60"/>
-      <c r="AW3" s="60"/>
-      <c r="AX3" s="60"/>
-      <c r="AY3" s="60"/>
-      <c r="AZ3" s="60"/>
-      <c r="BA3" s="60"/>
-      <c r="BC3" s="60" t="s">
+      <c r="AU3" s="50"/>
+      <c r="AV3" s="50"/>
+      <c r="AW3" s="50"/>
+      <c r="AX3" s="50"/>
+      <c r="AY3" s="50"/>
+      <c r="AZ3" s="50"/>
+      <c r="BA3" s="50"/>
+      <c r="BC3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="BD3" s="60"/>
-      <c r="BE3" s="60"/>
-      <c r="BF3" s="60"/>
-      <c r="BG3" s="60"/>
-      <c r="BH3" s="60"/>
-      <c r="BI3" s="60"/>
-      <c r="BJ3" s="60"/>
-      <c r="BL3" s="60" t="s">
+      <c r="BD3" s="50"/>
+      <c r="BE3" s="50"/>
+      <c r="BF3" s="50"/>
+      <c r="BG3" s="50"/>
+      <c r="BH3" s="50"/>
+      <c r="BI3" s="50"/>
+      <c r="BJ3" s="50"/>
+      <c r="BL3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="BM3" s="60"/>
-      <c r="BN3" s="60"/>
-      <c r="BO3" s="60"/>
-      <c r="BP3" s="60"/>
-      <c r="BQ3" s="60"/>
-      <c r="BR3" s="60"/>
-      <c r="BS3" s="60"/>
-      <c r="BU3" s="60" t="s">
+      <c r="BM3" s="50"/>
+      <c r="BN3" s="50"/>
+      <c r="BO3" s="50"/>
+      <c r="BP3" s="50"/>
+      <c r="BQ3" s="50"/>
+      <c r="BR3" s="50"/>
+      <c r="BS3" s="50"/>
+      <c r="BU3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="BV3" s="60"/>
-      <c r="BW3" s="60"/>
-      <c r="BX3" s="60"/>
-      <c r="BY3" s="60"/>
-      <c r="BZ3" s="60"/>
-      <c r="CA3" s="60"/>
-      <c r="CB3" s="60"/>
-      <c r="CD3" s="60" t="s">
+      <c r="BV3" s="50"/>
+      <c r="BW3" s="50"/>
+      <c r="BX3" s="50"/>
+      <c r="BY3" s="50"/>
+      <c r="BZ3" s="50"/>
+      <c r="CA3" s="50"/>
+      <c r="CB3" s="50"/>
+      <c r="CD3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="CE3" s="60"/>
-      <c r="CF3" s="60"/>
-      <c r="CG3" s="60"/>
-      <c r="CH3" s="60"/>
-      <c r="CI3" s="60"/>
-      <c r="CJ3" s="60"/>
-      <c r="CK3" s="60"/>
-      <c r="CM3" s="60" t="s">
+      <c r="CE3" s="50"/>
+      <c r="CF3" s="50"/>
+      <c r="CG3" s="50"/>
+      <c r="CH3" s="50"/>
+      <c r="CI3" s="50"/>
+      <c r="CJ3" s="50"/>
+      <c r="CK3" s="50"/>
+      <c r="CM3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="CN3" s="60"/>
-      <c r="CO3" s="60"/>
-      <c r="CP3" s="60"/>
-      <c r="CQ3" s="60"/>
-      <c r="CR3" s="60"/>
-      <c r="CS3" s="60"/>
-      <c r="CT3" s="60"/>
-      <c r="CV3" s="60" t="s">
+      <c r="CN3" s="50"/>
+      <c r="CO3" s="50"/>
+      <c r="CP3" s="50"/>
+      <c r="CQ3" s="50"/>
+      <c r="CR3" s="50"/>
+      <c r="CS3" s="50"/>
+      <c r="CT3" s="50"/>
+      <c r="CV3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="CW3" s="60"/>
-      <c r="CX3" s="60"/>
-      <c r="CY3" s="60"/>
-      <c r="CZ3" s="60"/>
-      <c r="DA3" s="60"/>
-      <c r="DB3" s="60"/>
-      <c r="DC3" s="60"/>
-      <c r="DE3" s="60" t="s">
+      <c r="CW3" s="50"/>
+      <c r="CX3" s="50"/>
+      <c r="CY3" s="50"/>
+      <c r="CZ3" s="50"/>
+      <c r="DA3" s="50"/>
+      <c r="DB3" s="50"/>
+      <c r="DC3" s="50"/>
+      <c r="DE3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="DF3" s="60"/>
-      <c r="DG3" s="60"/>
-      <c r="DH3" s="60"/>
-      <c r="DI3" s="60"/>
-      <c r="DJ3" s="60"/>
-      <c r="DK3" s="60"/>
-      <c r="DL3" s="60"/>
-      <c r="DN3" s="60" t="s">
+      <c r="DF3" s="50"/>
+      <c r="DG3" s="50"/>
+      <c r="DH3" s="50"/>
+      <c r="DI3" s="50"/>
+      <c r="DJ3" s="50"/>
+      <c r="DK3" s="50"/>
+      <c r="DL3" s="50"/>
+      <c r="DN3" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="DO3" s="60"/>
-      <c r="DP3" s="60"/>
-      <c r="DQ3" s="60"/>
-      <c r="DR3" s="60"/>
-      <c r="DS3" s="60"/>
-      <c r="DT3" s="60"/>
-      <c r="DU3" s="60"/>
+      <c r="DO3" s="50"/>
+      <c r="DP3" s="50"/>
+      <c r="DQ3" s="50"/>
+      <c r="DR3" s="50"/>
+      <c r="DS3" s="50"/>
+      <c r="DT3" s="50"/>
+      <c r="DU3" s="50"/>
     </row>
-    <row r="4" spans="1:125">
-      <c r="A4" s="61" t="s">
+    <row r="4" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="61"/>
+      <c r="B4" s="46"/>
       <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2313,10 +2319,10 @@
       <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="61" t="s">
+      <c r="J4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="61"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2335,10 +2341,10 @@
       <c r="Q4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S4" s="61" t="s">
+      <c r="S4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="T4" s="61"/>
+      <c r="T4" s="46"/>
       <c r="U4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2357,10 +2363,10 @@
       <c r="Z4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="61" t="s">
+      <c r="AB4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AC4" s="61"/>
+      <c r="AC4" s="46"/>
       <c r="AD4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2379,10 +2385,10 @@
       <c r="AI4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AK4" s="61" t="s">
+      <c r="AK4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AL4" s="61"/>
+      <c r="AL4" s="46"/>
       <c r="AM4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2401,10 +2407,10 @@
       <c r="AR4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AT4" s="61" t="s">
+      <c r="AT4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AU4" s="61"/>
+      <c r="AU4" s="46"/>
       <c r="AV4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2423,10 +2429,10 @@
       <c r="BA4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BC4" s="61" t="s">
+      <c r="BC4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="BD4" s="61"/>
+      <c r="BD4" s="46"/>
       <c r="BE4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2445,10 +2451,10 @@
       <c r="BJ4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BL4" s="61" t="s">
+      <c r="BL4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="BM4" s="61"/>
+      <c r="BM4" s="46"/>
       <c r="BN4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2467,10 +2473,10 @@
       <c r="BS4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BU4" s="61" t="s">
+      <c r="BU4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="BV4" s="61"/>
+      <c r="BV4" s="46"/>
       <c r="BW4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2489,10 +2495,10 @@
       <c r="CB4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="CD4" s="61" t="s">
+      <c r="CD4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="CE4" s="61"/>
+      <c r="CE4" s="46"/>
       <c r="CF4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2511,10 +2517,10 @@
       <c r="CK4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="CM4" s="61" t="s">
+      <c r="CM4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="CN4" s="61"/>
+      <c r="CN4" s="46"/>
       <c r="CO4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2533,10 +2539,10 @@
       <c r="CT4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="CV4" s="61" t="s">
+      <c r="CV4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="CW4" s="61"/>
+      <c r="CW4" s="46"/>
       <c r="CX4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2552,13 +2558,13 @@
       <c r="DB4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="DC4" s="35" t="s">
+      <c r="DC4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="DE4" s="61" t="s">
+      <c r="DE4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="DF4" s="61"/>
+      <c r="DF4" s="46"/>
       <c r="DG4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2574,13 +2580,13 @@
       <c r="DK4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="DL4" s="35" t="s">
+      <c r="DL4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="DN4" s="61" t="s">
+      <c r="DN4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="DO4" s="61"/>
+      <c r="DO4" s="46"/>
       <c r="DP4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2600,11 +2606,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:125" ht="18.75" customHeight="1">
-      <c r="A5" s="59" t="s">
+    <row r="5" spans="1:125" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="59"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2621,10 +2627,10 @@
       <c r="H5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="59"/>
+      <c r="K5" s="42"/>
       <c r="L5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2643,10 +2649,10 @@
       <c r="Q5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="S5" s="59" t="s">
+      <c r="S5" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="T5" s="59"/>
+      <c r="T5" s="42"/>
       <c r="U5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2665,10 +2671,10 @@
       <c r="Z5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AB5" s="59" t="s">
+      <c r="AB5" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="AC5" s="59"/>
+      <c r="AC5" s="42"/>
       <c r="AD5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2687,10 +2693,10 @@
       <c r="AI5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AK5" s="59" t="s">
+      <c r="AK5" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="AL5" s="59"/>
+      <c r="AL5" s="42"/>
       <c r="AM5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2707,10 +2713,10 @@
       <c r="AR5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AT5" s="59" t="s">
+      <c r="AT5" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="AU5" s="59"/>
+      <c r="AU5" s="42"/>
       <c r="AV5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2727,10 +2733,10 @@
       <c r="BA5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="BC5" s="59" t="s">
+      <c r="BC5" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="BD5" s="59"/>
+      <c r="BD5" s="42"/>
       <c r="BE5" s="2" t="s">
         <v>47</v>
       </c>
@@ -2747,10 +2753,10 @@
       <c r="BJ5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="BL5" s="59" t="s">
+      <c r="BL5" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="BM5" s="59"/>
+      <c r="BM5" s="42"/>
       <c r="BN5" s="2" t="s">
         <v>50</v>
       </c>
@@ -2767,10 +2773,10 @@
       <c r="BS5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="BU5" s="59" t="s">
+      <c r="BU5" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="BV5" s="59"/>
+      <c r="BV5" s="42"/>
       <c r="BW5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2785,12 +2791,12 @@
       </c>
       <c r="CA5" s="2"/>
       <c r="CB5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="CD5" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="CD5" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="CE5" s="59"/>
+      <c r="CE5" s="42"/>
       <c r="CF5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2805,12 +2811,12 @@
       </c>
       <c r="CJ5" s="2"/>
       <c r="CK5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="CM5" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="CM5" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="CN5" s="59"/>
+      <c r="CN5" s="42"/>
       <c r="CO5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2825,12 +2831,12 @@
       </c>
       <c r="CS5" s="2"/>
       <c r="CT5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="CV5" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="CV5" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="CW5" s="59"/>
+      <c r="CW5" s="42"/>
       <c r="CX5" s="2" t="s">
         <v>47</v>
       </c>
@@ -2843,14 +2849,14 @@
       <c r="DA5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="DB5" s="34"/>
-      <c r="DC5" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="DE5" s="59" t="s">
+      <c r="DB5" s="31"/>
+      <c r="DC5" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="DE5" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="DF5" s="59"/>
+      <c r="DF5" s="42"/>
       <c r="DG5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2863,14 +2869,14 @@
       <c r="DJ5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="DK5" s="34"/>
-      <c r="DL5" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="DN5" s="59" t="s">
+      <c r="DK5" s="31"/>
+      <c r="DL5" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="DN5" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="DO5" s="59"/>
+      <c r="DO5" s="42"/>
       <c r="DP5" s="2" t="s">
         <v>38</v>
       </c>
@@ -2885,19 +2891,19 @@
       </c>
       <c r="DT5" s="2"/>
       <c r="DU5" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:125" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="42"/>
+      <c r="C6" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:125" ht="18" customHeight="1">
-      <c r="A6" s="59" t="s">
+      <c r="D6" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>40</v>
@@ -2905,17 +2911,17 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="42"/>
+      <c r="L6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J6" s="59" t="s">
+      <c r="M6" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="K6" s="59"/>
-      <c r="L6" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>40</v>
@@ -2923,17 +2929,17 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="S6" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="T6" s="42"/>
+      <c r="U6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="S6" s="59" t="s">
+      <c r="V6" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="T6" s="59"/>
-      <c r="U6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="V6" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="W6" s="2" t="s">
         <v>40</v>
@@ -2941,17 +2947,17 @@
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB6" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC6" s="58"/>
+      <c r="AD6" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="AB6" s="62" t="s">
+      <c r="AE6" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="AC6" s="62"/>
-      <c r="AD6" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE6" s="11" t="s">
-        <v>72</v>
       </c>
       <c r="AF6" s="10" t="s">
         <v>40</v>
@@ -2959,12 +2965,12 @@
       <c r="AG6" s="10"/>
       <c r="AH6" s="10"/>
       <c r="AI6" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="AK6" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK6" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="AL6" s="62"/>
+      <c r="AL6" s="58"/>
       <c r="AM6" s="2" t="s">
         <v>38</v>
       </c>
@@ -2981,15 +2987,15 @@
       <c r="AR6" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="AT6" s="62" t="s">
+      <c r="AT6" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU6" s="58"/>
+      <c r="AV6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW6" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="AU6" s="62"/>
-      <c r="AV6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW6" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="AX6" s="10" t="s">
         <v>40</v>
@@ -2997,17 +3003,17 @@
       <c r="AY6" s="10"/>
       <c r="AZ6" s="10"/>
       <c r="BA6" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="BC6" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="BC6" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="BD6" s="58"/>
+      <c r="BE6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="BF6" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="BD6" s="62"/>
-      <c r="BE6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="BF6" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="BG6" s="10" t="s">
         <v>40</v>
@@ -3015,17 +3021,17 @@
       <c r="BH6" s="10"/>
       <c r="BI6" s="10"/>
       <c r="BJ6" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="BL6" s="59" t="s">
-        <v>78</v>
-      </c>
-      <c r="BM6" s="59"/>
+        <v>75</v>
+      </c>
+      <c r="BL6" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="BM6" s="42"/>
       <c r="BN6" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="BO6" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="BP6" s="2" t="s">
         <v>40</v>
@@ -3033,12 +3039,12 @@
       <c r="BQ6" s="2"/>
       <c r="BR6" s="2"/>
       <c r="BS6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="BU6" s="62" t="s">
-        <v>79</v>
-      </c>
-      <c r="BV6" s="62"/>
+        <v>67</v>
+      </c>
+      <c r="BU6" s="58" t="s">
+        <v>77</v>
+      </c>
+      <c r="BV6" s="58"/>
       <c r="BW6" s="2" t="s">
         <v>38</v>
       </c>
@@ -3053,12 +3059,12 @@
         <v>41</v>
       </c>
       <c r="CB6" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="CD6" s="62" t="s">
-        <v>81</v>
-      </c>
-      <c r="CE6" s="62"/>
+        <v>215</v>
+      </c>
+      <c r="CD6" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="CE6" s="58"/>
       <c r="CF6" s="2" t="s">
         <v>38</v>
       </c>
@@ -3073,12 +3079,12 @@
         <v>41</v>
       </c>
       <c r="CK6" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="CM6" s="62" t="s">
-        <v>81</v>
-      </c>
-      <c r="CN6" s="62"/>
+        <v>79</v>
+      </c>
+      <c r="CM6" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="CN6" s="58"/>
       <c r="CO6" s="2" t="s">
         <v>38</v>
       </c>
@@ -3089,34 +3095,34 @@
         <v>40</v>
       </c>
       <c r="CR6" s="10"/>
-      <c r="CS6" s="32" t="s">
+      <c r="CS6" s="29" t="s">
         <v>41</v>
       </c>
       <c r="CT6" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="CV6" s="62" t="s">
+        <v>219</v>
+      </c>
+      <c r="CV6" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="CW6" s="58"/>
+      <c r="CX6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="CY6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="CW6" s="62"/>
-      <c r="CX6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="CY6" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="CZ6" s="10" t="s">
         <v>40</v>
       </c>
       <c r="DA6" s="10"/>
-      <c r="DB6" s="32"/>
-      <c r="DC6" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="DE6" s="62" t="s">
-        <v>84</v>
-      </c>
-      <c r="DF6" s="62"/>
+      <c r="DB6" s="29"/>
+      <c r="DC6" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="DE6" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="DF6" s="58"/>
       <c r="DG6" s="2" t="s">
         <v>38</v>
       </c>
@@ -3127,16 +3133,16 @@
         <v>40</v>
       </c>
       <c r="DJ6" s="10"/>
-      <c r="DK6" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="DL6" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="DN6" s="62" t="s">
+      <c r="DK6" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="DL6" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="DN6" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="DO6" s="62"/>
+      <c r="DO6" s="58"/>
       <c r="DP6" s="2" t="s">
         <v>38</v>
       </c>
@@ -3151,19 +3157,19 @@
         <v>41</v>
       </c>
       <c r="DU6" s="10" t="s">
-        <v>86</v>
+        <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:125" ht="17.25" customHeight="1">
-      <c r="A7" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="B7" s="59"/>
+    <row r="7" spans="1:125" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="42"/>
       <c r="C7" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>40</v>
@@ -3171,37 +3177,37 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J7" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="72"/>
-      <c r="O7" s="72"/>
-      <c r="P7" s="72"/>
+        <v>85</v>
+      </c>
+      <c r="J7" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
       <c r="Q7" s="45"/>
-      <c r="S7" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="T7" s="72"/>
-      <c r="U7" s="72"/>
-      <c r="V7" s="72"/>
-      <c r="W7" s="72"/>
-      <c r="X7" s="72"/>
-      <c r="Y7" s="72"/>
+      <c r="S7" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="T7" s="44"/>
+      <c r="U7" s="44"/>
+      <c r="V7" s="44"/>
+      <c r="W7" s="44"/>
+      <c r="X7" s="44"/>
+      <c r="Y7" s="44"/>
       <c r="Z7" s="45"/>
-      <c r="AB7" s="55" t="s">
-        <v>92</v>
+      <c r="AB7" s="56" t="s">
+        <v>87</v>
       </c>
       <c r="AC7" s="57"/>
       <c r="AD7" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="AE7" s="9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="AF7" s="9" t="s">
         <v>40</v>
@@ -3209,17 +3215,17 @@
       <c r="AG7" s="9"/>
       <c r="AH7" s="9"/>
       <c r="AI7" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="AK7" s="55" t="s">
-        <v>96</v>
+        <v>90</v>
+      </c>
+      <c r="AK7" s="56" t="s">
+        <v>91</v>
       </c>
       <c r="AL7" s="57"/>
       <c r="AM7" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AN7" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AO7" s="9" t="s">
         <v>40</v>
@@ -3227,17 +3233,17 @@
       <c r="AP7" s="9"/>
       <c r="AQ7" s="20"/>
       <c r="AR7" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="AT7" s="55" t="s">
-        <v>98</v>
+        <v>92</v>
+      </c>
+      <c r="AT7" s="56" t="s">
+        <v>93</v>
       </c>
       <c r="AU7" s="57"/>
       <c r="AV7" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AW7" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AX7" s="9" t="s">
         <v>40</v>
@@ -3245,17 +3251,17 @@
       <c r="AY7" s="9"/>
       <c r="AZ7" s="20"/>
       <c r="BA7" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="BC7" s="55" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+      <c r="BC7" s="56" t="s">
+        <v>95</v>
       </c>
       <c r="BD7" s="57"/>
       <c r="BE7" s="9" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="BF7" s="13" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="BG7" s="9" t="s">
         <v>40</v>
@@ -3263,20 +3269,20 @@
       <c r="BH7" s="9"/>
       <c r="BI7" s="20"/>
       <c r="BJ7" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="BL7" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="BM7" s="72"/>
-      <c r="BN7" s="72"/>
-      <c r="BO7" s="72"/>
-      <c r="BP7" s="72"/>
-      <c r="BQ7" s="72"/>
-      <c r="BR7" s="72"/>
+        <v>98</v>
+      </c>
+      <c r="BL7" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="BM7" s="44"/>
+      <c r="BN7" s="44"/>
+      <c r="BO7" s="44"/>
+      <c r="BP7" s="44"/>
+      <c r="BQ7" s="44"/>
+      <c r="BR7" s="44"/>
       <c r="BS7" s="45"/>
-      <c r="BU7" s="55" t="s">
-        <v>104</v>
+      <c r="BU7" s="56" t="s">
+        <v>99</v>
       </c>
       <c r="BV7" s="57"/>
       <c r="BW7" s="9" t="s">
@@ -3293,10 +3299,10 @@
         <v>41</v>
       </c>
       <c r="CB7" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="CD7" s="55" t="s">
-        <v>106</v>
+        <v>216</v>
+      </c>
+      <c r="CD7" s="56" t="s">
+        <v>100</v>
       </c>
       <c r="CE7" s="57"/>
       <c r="CF7" s="9" t="s">
@@ -3313,10 +3319,10 @@
         <v>41</v>
       </c>
       <c r="CK7" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="CM7" s="55" t="s">
-        <v>108</v>
+        <v>221</v>
+      </c>
+      <c r="CM7" s="56" t="s">
+        <v>101</v>
       </c>
       <c r="CN7" s="57"/>
       <c r="CO7" s="9" t="s">
@@ -3333,28 +3339,28 @@
         <v>41</v>
       </c>
       <c r="CT7" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="CV7" s="55" t="s">
-        <v>100</v>
+        <v>220</v>
+      </c>
+      <c r="CV7" s="56" t="s">
+        <v>95</v>
       </c>
       <c r="CW7" s="57"/>
       <c r="CX7" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="CY7" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="CY7" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="CZ7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="DA7" s="9"/>
+      <c r="DB7" s="26"/>
+      <c r="DC7" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="CZ7" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="DA7" s="9"/>
-      <c r="DB7" s="29"/>
-      <c r="DC7" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="DE7" s="55" t="s">
-        <v>111</v>
+      <c r="DE7" s="56" t="s">
+        <v>103</v>
       </c>
       <c r="DF7" s="57"/>
       <c r="DG7" s="2" t="s">
@@ -3367,14 +3373,14 @@
         <v>40</v>
       </c>
       <c r="DJ7" s="9"/>
-      <c r="DK7" s="29" t="s">
+      <c r="DK7" s="26" t="s">
         <v>41</v>
       </c>
       <c r="DL7" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="DN7" s="55" t="s">
-        <v>84</v>
+        <v>223</v>
+      </c>
+      <c r="DN7" s="56" t="s">
+        <v>81</v>
       </c>
       <c r="DO7" s="57"/>
       <c r="DP7" s="9" t="s">
@@ -3391,19 +3397,19 @@
         <v>41</v>
       </c>
       <c r="DU7" s="9" t="s">
-        <v>82</v>
+        <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:125">
-      <c r="A8" s="59" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" s="59"/>
+    <row r="8" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="42"/>
       <c r="C8" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>40</v>
@@ -3411,53 +3417,53 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="J8" s="61" t="s">
-        <v>115</v>
-      </c>
-      <c r="K8" s="61"/>
+        <v>105</v>
+      </c>
+      <c r="J8" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="K8" s="46"/>
       <c r="L8" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="O8" s="61" t="s">
-        <v>119</v>
-      </c>
-      <c r="P8" s="61"/>
-      <c r="Q8" s="61"/>
-      <c r="S8" s="61" t="s">
-        <v>115</v>
-      </c>
-      <c r="T8" s="61"/>
+        <v>109</v>
+      </c>
+      <c r="O8" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="P8" s="46"/>
+      <c r="Q8" s="46"/>
+      <c r="S8" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="T8" s="46"/>
       <c r="U8" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="X8" s="61" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y8" s="61"/>
-      <c r="Z8" s="61"/>
-      <c r="AB8" s="55" t="s">
-        <v>120</v>
+        <v>109</v>
+      </c>
+      <c r="X8" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y8" s="46"/>
+      <c r="Z8" s="46"/>
+      <c r="AB8" s="56" t="s">
+        <v>111</v>
       </c>
       <c r="AC8" s="57"/>
       <c r="AD8" s="9" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="AE8" s="9" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="AF8" s="9" t="s">
         <v>40</v>
@@ -3465,17 +3471,17 @@
       <c r="AG8" s="9"/>
       <c r="AH8" s="9"/>
       <c r="AI8" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="AK8" s="55" t="s">
-        <v>124</v>
+        <v>114</v>
+      </c>
+      <c r="AK8" s="56" t="s">
+        <v>115</v>
       </c>
       <c r="AL8" s="57"/>
       <c r="AM8" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AN8" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AO8" s="9" t="s">
         <v>40</v>
@@ -3483,17 +3489,17 @@
       <c r="AP8" s="9"/>
       <c r="AQ8" s="9"/>
       <c r="AR8" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="AT8" s="55" t="s">
-        <v>126</v>
+        <v>116</v>
+      </c>
+      <c r="AT8" s="56" t="s">
+        <v>117</v>
       </c>
       <c r="AU8" s="57"/>
       <c r="AV8" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AW8" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AX8" s="9" t="s">
         <v>40</v>
@@ -3501,17 +3507,17 @@
       <c r="AY8" s="9"/>
       <c r="AZ8" s="9"/>
       <c r="BA8" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="BC8" s="63" t="s">
-        <v>128</v>
-      </c>
-      <c r="BD8" s="64"/>
+        <v>118</v>
+      </c>
+      <c r="BC8" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="BD8" s="63"/>
       <c r="BE8" s="12" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="BF8" s="14" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="BG8" s="12" t="s">
         <v>40</v>
@@ -3519,35 +3525,35 @@
       <c r="BH8" s="12"/>
       <c r="BI8" s="12"/>
       <c r="BJ8" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="BL8" s="61" t="s">
-        <v>115</v>
-      </c>
-      <c r="BM8" s="61"/>
+        <v>122</v>
+      </c>
+      <c r="BL8" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="BM8" s="46"/>
       <c r="BN8" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="BO8" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="BP8" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="BQ8" s="61" t="s">
-        <v>119</v>
-      </c>
-      <c r="BR8" s="61"/>
-      <c r="BS8" s="61"/>
-      <c r="BU8" s="55" t="s">
-        <v>132</v>
+        <v>109</v>
+      </c>
+      <c r="BQ8" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="BR8" s="46"/>
+      <c r="BS8" s="46"/>
+      <c r="BU8" s="56" t="s">
+        <v>123</v>
       </c>
       <c r="BV8" s="57"/>
       <c r="BW8" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="BX8" s="13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BY8" s="9" t="s">
         <v>40</v>
@@ -3555,17 +3561,17 @@
       <c r="BZ8" s="9"/>
       <c r="CA8" s="9"/>
       <c r="CB8" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="CD8" s="55" t="s">
-        <v>134</v>
+        <v>124</v>
+      </c>
+      <c r="CD8" s="56" t="s">
+        <v>125</v>
       </c>
       <c r="CE8" s="57"/>
-      <c r="CF8" s="28" t="s">
-        <v>71</v>
+      <c r="CF8" s="25" t="s">
+        <v>69</v>
       </c>
       <c r="CG8" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="CH8" s="9" t="s">
         <v>40</v>
@@ -3573,30 +3579,30 @@
       <c r="CI8" s="9"/>
       <c r="CJ8" s="9"/>
       <c r="CK8" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="CM8" s="63" t="s">
-        <v>136</v>
-      </c>
-      <c r="CN8" s="64"/>
-      <c r="CO8" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="CM8" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="CN8" s="63"/>
+      <c r="CO8" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="CP8" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="CQ8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="CR8" s="12"/>
+      <c r="CS8" s="26"/>
+      <c r="CT8" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="CV8" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="CP8" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="CQ8" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="CR8" s="12"/>
-      <c r="CS8" s="29"/>
-      <c r="CT8" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="CV8" s="63" t="s">
-        <v>138</v>
-      </c>
-      <c r="CW8" s="64"/>
+      <c r="CW8" s="63"/>
       <c r="CX8" s="12" t="s">
         <v>38</v>
       </c>
@@ -3606,15 +3612,15 @@
       <c r="CZ8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="DA8" s="29"/>
+      <c r="DA8" s="26"/>
       <c r="DB8" s="9"/>
       <c r="DC8" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="DE8" s="63" t="s">
-        <v>140</v>
-      </c>
-      <c r="DF8" s="64"/>
+        <v>130</v>
+      </c>
+      <c r="DE8" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="DF8" s="63"/>
       <c r="DG8" s="12" t="s">
         <v>38</v>
       </c>
@@ -3624,20 +3630,20 @@
       <c r="DI8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="DJ8" s="29"/>
+      <c r="DJ8" s="26"/>
       <c r="DK8" s="9"/>
       <c r="DL8" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="DN8" s="55" t="s">
-        <v>142</v>
+        <v>132</v>
+      </c>
+      <c r="DN8" s="56" t="s">
+        <v>133</v>
       </c>
       <c r="DO8" s="57"/>
       <c r="DP8" s="9" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="DQ8" s="13" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="DR8" s="9" t="s">
         <v>40</v>
@@ -3645,79 +3651,79 @@
       <c r="DS8" s="9"/>
       <c r="DT8" s="9"/>
       <c r="DU8" s="21" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:125" ht="15.75" customHeight="1">
-      <c r="A9" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="J9" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="K9" s="43"/>
-      <c r="L9" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="O9" s="42" t="s">
+    <row r="9" spans="1:125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="J9" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="K9" s="54"/>
+      <c r="L9" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="P9" s="50"/>
-      <c r="Q9" s="43"/>
-      <c r="S9" s="42" t="s">
-        <v>147</v>
-      </c>
-      <c r="T9" s="43"/>
-      <c r="U9" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="V9" s="40"/>
-      <c r="W9" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="X9" s="42" t="s">
+      <c r="P9" s="55"/>
+      <c r="Q9" s="54"/>
+      <c r="S9" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="T9" s="54"/>
+      <c r="U9" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="X9" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="Y9" s="50"/>
-      <c r="Z9" s="43"/>
-      <c r="AB9" s="55" t="s">
-        <v>148</v>
-      </c>
-      <c r="AC9" s="57"/>
-      <c r="AD9" s="9" t="s">
-        <v>129</v>
+      <c r="Y9" s="55"/>
+      <c r="Z9" s="54"/>
+      <c r="AB9" s="62" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC9" s="63"/>
+      <c r="AD9" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="AE9" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="AF9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG9" s="9"/>
-      <c r="AH9" s="9"/>
-      <c r="AI9" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="AK9" s="63" t="s">
-        <v>150</v>
-      </c>
-      <c r="AL9" s="64"/>
+        <v>121</v>
+      </c>
+      <c r="AF9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG9" s="12"/>
+      <c r="AH9" s="12"/>
+      <c r="AI9" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK9" s="62" t="s">
+        <v>141</v>
+      </c>
+      <c r="AL9" s="63"/>
       <c r="AM9" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AN9" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AO9" s="12" t="s">
         <v>40</v>
@@ -3725,17 +3731,17 @@
       <c r="AP9" s="12"/>
       <c r="AQ9" s="12"/>
       <c r="AR9" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="AT9" s="63" t="s">
-        <v>152</v>
-      </c>
-      <c r="AU9" s="64"/>
+        <v>142</v>
+      </c>
+      <c r="AT9" s="62" t="s">
+        <v>143</v>
+      </c>
+      <c r="AU9" s="63"/>
       <c r="AV9" s="12" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="AW9" s="14" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="AX9" s="12" t="s">
         <v>40</v>
@@ -3743,22 +3749,22 @@
       <c r="AY9" s="12"/>
       <c r="AZ9" s="12"/>
       <c r="BA9" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="BC9" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="BD9" s="53"/>
+        <v>146</v>
+      </c>
+      <c r="BC9" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="BD9" s="66"/>
       <c r="BE9" s="22"/>
       <c r="BF9" s="22"/>
       <c r="BG9" s="22"/>
       <c r="BH9" s="22"/>
       <c r="BI9" s="22"/>
       <c r="BJ9" s="22"/>
-      <c r="BL9" s="69" t="s">
-        <v>156</v>
-      </c>
-      <c r="BM9" s="70"/>
+      <c r="BL9" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="BM9" s="48"/>
       <c r="BN9" s="4" t="s">
         <v>41</v>
       </c>
@@ -3766,102 +3772,102 @@
       <c r="BP9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="BQ9" s="69" t="s">
+      <c r="BQ9" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="BR9" s="71"/>
-      <c r="BS9" s="70"/>
-      <c r="BU9" s="63" t="s">
-        <v>157</v>
-      </c>
-      <c r="BV9" s="64"/>
+      <c r="BR9" s="49"/>
+      <c r="BS9" s="48"/>
+      <c r="BU9" s="62" t="s">
+        <v>148</v>
+      </c>
+      <c r="BV9" s="63"/>
       <c r="BW9" s="12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="BX9" s="13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BY9" s="12" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="BZ9" s="12"/>
       <c r="CA9" s="12"/>
       <c r="CB9" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="CD9" s="63" t="s">
-        <v>160</v>
-      </c>
-      <c r="CE9" s="64"/>
+        <v>150</v>
+      </c>
+      <c r="CD9" s="62" t="s">
+        <v>151</v>
+      </c>
+      <c r="CE9" s="63"/>
       <c r="CF9" s="12" t="s">
         <v>47</v>
       </c>
       <c r="CG9" s="13" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="CH9" s="12" t="s">
         <v>40</v>
       </c>
       <c r="CI9" s="12"/>
-      <c r="CJ9" s="29"/>
+      <c r="CJ9" s="26"/>
       <c r="CK9" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="CM9" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="CN9" s="54"/>
-      <c r="CO9" s="54"/>
-      <c r="CP9" s="54"/>
-      <c r="CQ9" s="54"/>
-      <c r="CR9" s="54"/>
-      <c r="CS9" s="54"/>
-      <c r="CT9" s="68"/>
-      <c r="CV9" s="49" t="s">
-        <v>163</v>
-      </c>
-      <c r="CW9" s="49"/>
+        <v>153</v>
+      </c>
+      <c r="CM9" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="CN9" s="68"/>
+      <c r="CO9" s="68"/>
+      <c r="CP9" s="68"/>
+      <c r="CQ9" s="68"/>
+      <c r="CR9" s="68"/>
+      <c r="CS9" s="68"/>
+      <c r="CT9" s="69"/>
+      <c r="CV9" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="CW9" s="40"/>
       <c r="CX9" s="9" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="CY9" s="13" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="CZ9" s="9" t="s">
         <v>40</v>
       </c>
       <c r="DA9" s="9"/>
-      <c r="DB9" s="36"/>
+      <c r="DB9" s="33"/>
       <c r="DC9" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="DE9" s="49" t="s">
-        <v>163</v>
-      </c>
-      <c r="DF9" s="49"/>
+        <v>155</v>
+      </c>
+      <c r="DE9" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="DF9" s="40"/>
       <c r="DG9" s="9" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="DH9" s="13" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="DI9" s="9" t="s">
         <v>40</v>
       </c>
       <c r="DJ9" s="9"/>
-      <c r="DK9" s="36"/>
+      <c r="DK9" s="33"/>
       <c r="DL9" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="DN9" s="63" t="s">
-        <v>166</v>
-      </c>
-      <c r="DO9" s="64"/>
+        <v>156</v>
+      </c>
+      <c r="DN9" s="62" t="s">
+        <v>157</v>
+      </c>
+      <c r="DO9" s="63"/>
       <c r="DP9" s="12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="DQ9" s="13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="DR9" s="12" t="s">
         <v>40</v>
@@ -3869,32 +3875,32 @@
       <c r="DS9" s="12"/>
       <c r="DT9" s="12"/>
       <c r="DU9" s="12" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:125">
-      <c r="A10" s="61" t="s">
-        <v>115</v>
-      </c>
-      <c r="B10" s="61"/>
+    <row r="10" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A10" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="46"/>
       <c r="C10" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F10" s="61" t="s">
-        <v>119</v>
-      </c>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="J10" s="49" t="s">
-        <v>168</v>
-      </c>
-      <c r="K10" s="49"/>
+        <v>109</v>
+      </c>
+      <c r="F10" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="J10" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="K10" s="40"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9" t="s">
         <v>41</v>
@@ -3902,15 +3908,15 @@
       <c r="N10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="O10" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="49"/>
-      <c r="S10" s="49" t="s">
-        <v>169</v>
-      </c>
-      <c r="T10" s="49"/>
+      <c r="O10" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="S10" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="T10" s="40"/>
       <c r="U10" s="9"/>
       <c r="V10" s="9" t="s">
         <v>41</v>
@@ -3918,30 +3924,30 @@
       <c r="W10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="X10" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y10" s="49"/>
-      <c r="Z10" s="49"/>
-      <c r="AB10" s="66" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC10" s="73"/>
-      <c r="AD10" s="73"/>
-      <c r="AE10" s="73"/>
-      <c r="AF10" s="73"/>
-      <c r="AG10" s="73"/>
-      <c r="AH10" s="73"/>
-      <c r="AI10" s="67"/>
-      <c r="AK10" s="55" t="s">
-        <v>170</v>
+      <c r="X10" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y10" s="40"/>
+      <c r="Z10" s="40"/>
+      <c r="AB10" s="76" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC10" s="76"/>
+      <c r="AD10" s="76"/>
+      <c r="AE10" s="76"/>
+      <c r="AF10" s="76"/>
+      <c r="AG10" s="76"/>
+      <c r="AH10" s="76"/>
+      <c r="AI10" s="76"/>
+      <c r="AK10" s="56" t="s">
+        <v>161</v>
       </c>
       <c r="AL10" s="57"/>
       <c r="AM10" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AN10" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AO10" s="9" t="s">
         <v>40</v>
@@ -3949,17 +3955,17 @@
       <c r="AP10" s="9"/>
       <c r="AQ10" s="9"/>
       <c r="AR10" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="AT10" s="55" t="s">
-        <v>172</v>
+        <v>162</v>
+      </c>
+      <c r="AT10" s="56" t="s">
+        <v>163</v>
       </c>
       <c r="AU10" s="57"/>
       <c r="AV10" s="12" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="AW10" s="14" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="AX10" s="9" t="s">
         <v>40</v>
@@ -3967,35 +3973,35 @@
       <c r="AY10" s="9"/>
       <c r="AZ10" s="9"/>
       <c r="BA10" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="BC10" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="BD10" s="48"/>
+        <v>166</v>
+      </c>
+      <c r="BC10" s="71" t="s">
+        <v>106</v>
+      </c>
+      <c r="BD10" s="73"/>
       <c r="BE10" s="24" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="BF10" s="24" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="BG10" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="BH10" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="BI10" s="47"/>
-      <c r="BJ10" s="48"/>
-      <c r="BU10" s="63" t="s">
-        <v>176</v>
-      </c>
-      <c r="BV10" s="64"/>
+        <v>109</v>
+      </c>
+      <c r="BH10" s="71" t="s">
+        <v>110</v>
+      </c>
+      <c r="BI10" s="72"/>
+      <c r="BJ10" s="73"/>
+      <c r="BU10" s="62" t="s">
+        <v>167</v>
+      </c>
+      <c r="BV10" s="63"/>
       <c r="BW10" s="12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="BX10" s="13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="BY10" s="12" t="s">
         <v>40</v>
@@ -4003,17 +4009,17 @@
       <c r="BZ10" s="12"/>
       <c r="CA10" s="12"/>
       <c r="CB10" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="CD10" s="49" t="s">
-        <v>178</v>
-      </c>
-      <c r="CE10" s="49"/>
+        <v>168</v>
+      </c>
+      <c r="CD10" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="CE10" s="40"/>
       <c r="CF10" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="CG10" s="30" t="s">
-        <v>180</v>
+        <v>170</v>
+      </c>
+      <c r="CG10" s="27" t="s">
+        <v>171</v>
       </c>
       <c r="CH10" s="9" t="s">
         <v>40</v>
@@ -4021,55 +4027,55 @@
       <c r="CI10" s="9"/>
       <c r="CJ10" s="9"/>
       <c r="CK10" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="CM10" s="66" t="s">
-        <v>115</v>
-      </c>
-      <c r="CN10" s="67"/>
+        <v>172</v>
+      </c>
+      <c r="CM10" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="CN10" s="61"/>
       <c r="CO10" s="24" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="CP10" s="24" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="CQ10" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="CR10" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="CS10" s="16"/>
-      <c r="CT10" s="17"/>
-      <c r="CV10" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="CW10" s="52"/>
-      <c r="CX10" s="52"/>
-      <c r="CY10" s="52"/>
-      <c r="CZ10" s="52"/>
-      <c r="DA10" s="52"/>
-      <c r="DB10" s="52"/>
-      <c r="DC10" s="53"/>
-      <c r="DE10" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="DF10" s="52"/>
-      <c r="DG10" s="52"/>
-      <c r="DH10" s="52"/>
-      <c r="DI10" s="52"/>
-      <c r="DJ10" s="52"/>
-      <c r="DK10" s="52"/>
-      <c r="DL10" s="53"/>
-      <c r="DN10" s="63" t="s">
-        <v>178</v>
-      </c>
-      <c r="DO10" s="64"/>
+        <v>109</v>
+      </c>
+      <c r="CR10" s="71" t="s">
+        <v>110</v>
+      </c>
+      <c r="CS10" s="72"/>
+      <c r="CT10" s="73"/>
+      <c r="CV10" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="CW10" s="74"/>
+      <c r="CX10" s="74"/>
+      <c r="CY10" s="74"/>
+      <c r="CZ10" s="74"/>
+      <c r="DA10" s="74"/>
+      <c r="DB10" s="74"/>
+      <c r="DC10" s="66"/>
+      <c r="DE10" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="DF10" s="74"/>
+      <c r="DG10" s="74"/>
+      <c r="DH10" s="74"/>
+      <c r="DI10" s="74"/>
+      <c r="DJ10" s="74"/>
+      <c r="DK10" s="74"/>
+      <c r="DL10" s="66"/>
+      <c r="DN10" s="62" t="s">
+        <v>169</v>
+      </c>
+      <c r="DO10" s="63"/>
       <c r="DP10" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="DQ10" s="30" t="s">
-        <v>102</v>
+        <v>96</v>
+      </c>
+      <c r="DQ10" s="27" t="s">
+        <v>97</v>
       </c>
       <c r="DR10" s="12" t="s">
         <v>40</v>
@@ -4077,14 +4083,14 @@
       <c r="DS10" s="12"/>
       <c r="DT10" s="12"/>
       <c r="DU10" s="12" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:125">
-      <c r="A11" s="75" t="s">
-        <v>183</v>
-      </c>
-      <c r="B11" s="75"/>
+    <row r="11" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A11" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="B11" s="52"/>
       <c r="C11" s="8" t="s">
         <v>41</v>
       </c>
@@ -4092,38 +4098,38 @@
       <c r="E11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="75" t="s">
+      <c r="F11" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="AB11" s="61" t="s">
-        <v>115</v>
-      </c>
-      <c r="AC11" s="61"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="AB11" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC11" s="46"/>
       <c r="AD11" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="AF11" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AG11" s="61" t="s">
-        <v>119</v>
-      </c>
-      <c r="AH11" s="61"/>
-      <c r="AI11" s="61"/>
-      <c r="AK11" s="55" t="s">
-        <v>184</v>
+        <v>109</v>
+      </c>
+      <c r="AG11" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH11" s="46"/>
+      <c r="AI11" s="46"/>
+      <c r="AK11" s="56" t="s">
+        <v>175</v>
       </c>
       <c r="AL11" s="57"/>
       <c r="AM11" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AN11" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AO11" s="12" t="s">
         <v>40</v>
@@ -4131,17 +4137,17 @@
       <c r="AP11" s="9"/>
       <c r="AQ11" s="9"/>
       <c r="AR11" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="AT11" s="63" t="s">
-        <v>186</v>
-      </c>
-      <c r="AU11" s="64"/>
+        <v>176</v>
+      </c>
+      <c r="AT11" s="62" t="s">
+        <v>177</v>
+      </c>
+      <c r="AU11" s="63"/>
       <c r="AV11" s="12" t="s">
         <v>38</v>
       </c>
       <c r="AW11" s="14" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="AX11" s="12" t="s">
         <v>40</v>
@@ -4149,12 +4155,12 @@
       <c r="AY11" s="12"/>
       <c r="AZ11" s="12"/>
       <c r="BA11" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="BC11" s="69" t="s">
-        <v>189</v>
-      </c>
-      <c r="BD11" s="70"/>
+        <v>213</v>
+      </c>
+      <c r="BC11" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="BD11" s="48"/>
       <c r="BE11" s="4" t="s">
         <v>41</v>
       </c>
@@ -4162,20 +4168,20 @@
       <c r="BG11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="BH11" s="69" t="s">
+      <c r="BH11" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="BI11" s="71"/>
-      <c r="BJ11" s="70"/>
-      <c r="BU11" s="49" t="s">
-        <v>190</v>
-      </c>
-      <c r="BV11" s="49"/>
+      <c r="BI11" s="49"/>
+      <c r="BJ11" s="48"/>
+      <c r="BU11" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="BV11" s="40"/>
       <c r="BW11" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="BX11" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="BY11" s="9" t="s">
         <v>40</v>
@@ -4183,10 +4189,10 @@
       <c r="BZ11" s="9"/>
       <c r="CA11" s="9"/>
       <c r="CB11" s="9" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="CD11" s="15" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="CE11" s="16"/>
       <c r="CF11" s="16"/>
@@ -4195,82 +4201,82 @@
       <c r="CI11" s="16"/>
       <c r="CJ11" s="16"/>
       <c r="CK11" s="17"/>
-      <c r="CM11" s="42" t="s">
-        <v>192</v>
-      </c>
-      <c r="CN11" s="43"/>
-      <c r="CO11" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="CP11" s="40"/>
-      <c r="CQ11" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="CR11" s="37" t="s">
+      <c r="CM11" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="CN11" s="54"/>
+      <c r="CO11" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="CP11" s="37"/>
+      <c r="CQ11" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="CR11" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="CS11" s="41"/>
-      <c r="CT11" s="38"/>
-      <c r="CV11" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="CW11" s="58"/>
+      <c r="CS11" s="38"/>
+      <c r="CT11" s="35"/>
+      <c r="CV11" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="CW11" s="64"/>
       <c r="CX11" s="24" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="CY11" s="24" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="CZ11" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="DA11" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="DB11" s="58"/>
-      <c r="DC11" s="58"/>
-      <c r="DE11" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="DF11" s="58"/>
+        <v>109</v>
+      </c>
+      <c r="DA11" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="DB11" s="64"/>
+      <c r="DC11" s="64"/>
+      <c r="DE11" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="DF11" s="64"/>
       <c r="DG11" s="24" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="DH11" s="24" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="DI11" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="DJ11" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="DK11" s="58"/>
-      <c r="DL11" s="58"/>
-      <c r="DN11" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="DO11" s="47"/>
-      <c r="DP11" s="47"/>
-      <c r="DQ11" s="47"/>
-      <c r="DR11" s="47"/>
-      <c r="DS11" s="47"/>
-      <c r="DT11" s="47"/>
-      <c r="DU11" s="48"/>
+        <v>109</v>
+      </c>
+      <c r="DJ11" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="DK11" s="64"/>
+      <c r="DL11" s="64"/>
+      <c r="DN11" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="DO11" s="72"/>
+      <c r="DP11" s="72"/>
+      <c r="DQ11" s="72"/>
+      <c r="DR11" s="72"/>
+      <c r="DS11" s="72"/>
+      <c r="DT11" s="72"/>
+      <c r="DU11" s="73"/>
     </row>
-    <row r="12" spans="1:125" ht="16.5" customHeight="1">
-      <c r="A12" s="74"/>
-      <c r="B12" s="74"/>
+    <row r="12" spans="1:125" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="51"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="AB12" s="69" t="s">
-        <v>193</v>
-      </c>
-      <c r="AC12" s="70"/>
+      <c r="AB12" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="AC12" s="48"/>
       <c r="AD12" s="4" t="s">
         <v>41</v>
       </c>
@@ -4278,20 +4284,20 @@
       <c r="AF12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AG12" s="69" t="s">
+      <c r="AG12" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="AH12" s="71"/>
-      <c r="AI12" s="70"/>
-      <c r="AK12" s="55" t="s">
-        <v>194</v>
+      <c r="AH12" s="49"/>
+      <c r="AI12" s="48"/>
+      <c r="AK12" s="56" t="s">
+        <v>183</v>
       </c>
       <c r="AL12" s="57"/>
       <c r="AM12" s="9" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="AN12" s="13" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="AO12" s="12" t="s">
         <v>40</v>
@@ -4299,27 +4305,27 @@
       <c r="AP12" s="9"/>
       <c r="AQ12" s="9"/>
       <c r="AR12" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="AT12" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="AU12" s="54"/>
-      <c r="AV12" s="54"/>
-      <c r="AW12" s="54"/>
-      <c r="AX12" s="54"/>
-      <c r="AY12" s="54"/>
-      <c r="AZ12" s="54"/>
-      <c r="BA12" s="54"/>
-      <c r="BU12" s="63" t="s">
-        <v>78</v>
-      </c>
-      <c r="BV12" s="64"/>
+        <v>212</v>
+      </c>
+      <c r="AT12" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU12" s="68"/>
+      <c r="AV12" s="68"/>
+      <c r="AW12" s="68"/>
+      <c r="AX12" s="68"/>
+      <c r="AY12" s="68"/>
+      <c r="AZ12" s="68"/>
+      <c r="BA12" s="68"/>
+      <c r="BU12" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="BV12" s="63"/>
       <c r="BW12" s="12" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="BX12" s="12" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="BY12" s="12" t="s">
         <v>40</v>
@@ -4327,44 +4333,44 @@
       <c r="BZ12" s="12"/>
       <c r="CA12" s="12"/>
       <c r="CB12" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="CD12" s="44" t="s">
-        <v>115</v>
+        <v>186</v>
+      </c>
+      <c r="CD12" s="43" t="s">
+        <v>106</v>
       </c>
       <c r="CE12" s="45"/>
       <c r="CF12" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="CG12" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="CH12" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="CI12" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="CJ12" s="72"/>
+        <v>109</v>
+      </c>
+      <c r="CI12" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="CJ12" s="44"/>
       <c r="CK12" s="45"/>
-      <c r="CM12" s="49" t="s">
-        <v>199</v>
-      </c>
-      <c r="CN12" s="49"/>
+      <c r="CM12" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="CN12" s="40"/>
       <c r="CO12" s="9"/>
       <c r="CP12" s="9" t="s">
         <v>41</v>
       </c>
       <c r="CQ12" s="9"/>
-      <c r="CR12" s="49" t="s">
-        <v>200</v>
-      </c>
-      <c r="CS12" s="49"/>
-      <c r="CT12" s="49"/>
-      <c r="CV12" s="69" t="s">
-        <v>201</v>
-      </c>
-      <c r="CW12" s="70"/>
+      <c r="CR12" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="CS12" s="40"/>
+      <c r="CT12" s="40"/>
+      <c r="CV12" s="47" t="s">
+        <v>189</v>
+      </c>
+      <c r="CW12" s="48"/>
       <c r="CX12" s="4" t="s">
         <v>41</v>
       </c>
@@ -4372,64 +4378,64 @@
       <c r="CZ12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="DA12" s="69" t="s">
+      <c r="DA12" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="DB12" s="71"/>
-      <c r="DC12" s="70"/>
-      <c r="DE12" s="42" t="s">
-        <v>202</v>
-      </c>
-      <c r="DF12" s="43"/>
-      <c r="DG12" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="DH12" s="40"/>
-      <c r="DI12" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="DJ12" s="42" t="s">
+      <c r="DB12" s="49"/>
+      <c r="DC12" s="48"/>
+      <c r="DE12" s="53" t="s">
+        <v>190</v>
+      </c>
+      <c r="DF12" s="54"/>
+      <c r="DG12" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="DH12" s="37"/>
+      <c r="DI12" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="DJ12" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="DK12" s="50"/>
-      <c r="DL12" s="43"/>
-      <c r="DN12" s="44" t="s">
-        <v>115</v>
+      <c r="DK12" s="55"/>
+      <c r="DL12" s="54"/>
+      <c r="DN12" s="43" t="s">
+        <v>106</v>
       </c>
       <c r="DO12" s="45"/>
       <c r="DP12" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="DQ12" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="DR12" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="DS12" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="DT12" s="26"/>
-      <c r="DU12" s="27"/>
+        <v>109</v>
+      </c>
+      <c r="DS12" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="DT12" s="78"/>
+      <c r="DU12" s="79"/>
     </row>
-    <row r="13" spans="1:125">
-      <c r="A13" s="74"/>
-      <c r="B13" s="74"/>
+    <row r="13" spans="1:125" x14ac:dyDescent="0.25">
+      <c r="A13" s="51"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="AK13" s="55" t="s">
-        <v>203</v>
+      <c r="AK13" s="56" t="s">
+        <v>191</v>
       </c>
       <c r="AL13" s="57"/>
       <c r="AM13" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="AN13" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="AO13" s="9" t="s">
         <v>40</v>
@@ -4437,35 +4443,35 @@
       <c r="AP13" s="19"/>
       <c r="AQ13" s="9"/>
       <c r="AR13" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="AT13" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="AU13" s="58"/>
+        <v>192</v>
+      </c>
+      <c r="AT13" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="AU13" s="64"/>
       <c r="AV13" s="24" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="AW13" s="24" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="AX13" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="AY13" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="AZ13" s="58"/>
-      <c r="BA13" s="58"/>
-      <c r="BU13" s="55" t="s">
-        <v>205</v>
+        <v>109</v>
+      </c>
+      <c r="AY13" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="AZ13" s="64"/>
+      <c r="BA13" s="64"/>
+      <c r="BU13" s="56" t="s">
+        <v>193</v>
       </c>
       <c r="BV13" s="57"/>
       <c r="BW13" s="9" t="s">
         <v>50</v>
       </c>
       <c r="BX13" s="9" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="BY13" s="9" t="s">
         <v>40</v>
@@ -4473,144 +4479,144 @@
       <c r="BZ13" s="9"/>
       <c r="CA13" s="9"/>
       <c r="CB13" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="CD13" s="42" t="s">
-        <v>208</v>
-      </c>
-      <c r="CE13" s="43"/>
-      <c r="CF13" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="CG13" s="40"/>
-      <c r="CH13" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="CI13" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="CD13" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="CE13" s="54"/>
+      <c r="CF13" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="CG13" s="37"/>
+      <c r="CH13" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="CI13" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="CJ13" s="41"/>
-      <c r="CK13" s="38"/>
-      <c r="DE13" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="DF13" s="49"/>
+      <c r="CJ13" s="38"/>
+      <c r="CK13" s="35"/>
+      <c r="DE13" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="DF13" s="40"/>
       <c r="DG13" s="9"/>
       <c r="DH13" s="9" t="s">
         <v>41</v>
       </c>
       <c r="DI13" s="9"/>
-      <c r="DJ13" s="49" t="s">
-        <v>210</v>
-      </c>
-      <c r="DK13" s="49"/>
-      <c r="DL13" s="49"/>
-      <c r="DN13" s="42" t="s">
-        <v>211</v>
-      </c>
-      <c r="DO13" s="43"/>
-      <c r="DP13" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="DQ13" s="40"/>
-      <c r="DR13" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="DS13" s="42" t="s">
+      <c r="DJ13" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="DK13" s="40"/>
+      <c r="DL13" s="40"/>
+      <c r="DN13" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="DO13" s="54"/>
+      <c r="DP13" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="DQ13" s="37"/>
+      <c r="DR13" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="DS13" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="DT13" s="50"/>
-      <c r="DU13" s="43"/>
+      <c r="DT13" s="55"/>
+      <c r="DU13" s="54"/>
     </row>
-    <row r="14" spans="1:125" ht="15" customHeight="1">
-      <c r="AK14" s="66" t="s">
-        <v>91</v>
-      </c>
-      <c r="AL14" s="73"/>
-      <c r="AM14" s="73"/>
-      <c r="AN14" s="73"/>
-      <c r="AO14" s="73"/>
-      <c r="AP14" s="73"/>
-      <c r="AQ14" s="73"/>
-      <c r="AR14" s="67"/>
-      <c r="AT14" s="42" t="s">
-        <v>212</v>
-      </c>
-      <c r="AU14" s="43"/>
-      <c r="AV14" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="AW14" s="40"/>
-      <c r="AX14" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="AY14" s="42" t="s">
+    <row r="14" spans="1:125" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AK14" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL14" s="60"/>
+      <c r="AM14" s="60"/>
+      <c r="AN14" s="60"/>
+      <c r="AO14" s="60"/>
+      <c r="AP14" s="60"/>
+      <c r="AQ14" s="60"/>
+      <c r="AR14" s="61"/>
+      <c r="AT14" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="AU14" s="54"/>
+      <c r="AV14" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW14" s="37"/>
+      <c r="AX14" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY14" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="AZ14" s="50"/>
-      <c r="BA14" s="43"/>
-      <c r="BU14" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="BV14" s="47"/>
-      <c r="BW14" s="47"/>
-      <c r="BX14" s="47"/>
-      <c r="BY14" s="47"/>
-      <c r="BZ14" s="47"/>
-      <c r="CA14" s="47"/>
-      <c r="CB14" s="48"/>
-      <c r="CD14" s="49" t="s">
-        <v>213</v>
-      </c>
-      <c r="CE14" s="49"/>
+      <c r="AZ14" s="55"/>
+      <c r="BA14" s="54"/>
+      <c r="BU14" s="71" t="s">
+        <v>86</v>
+      </c>
+      <c r="BV14" s="72"/>
+      <c r="BW14" s="72"/>
+      <c r="BX14" s="72"/>
+      <c r="BY14" s="72"/>
+      <c r="BZ14" s="72"/>
+      <c r="CA14" s="72"/>
+      <c r="CB14" s="73"/>
+      <c r="CD14" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="CE14" s="40"/>
       <c r="CF14" s="9"/>
       <c r="CG14" s="9" t="s">
         <v>41</v>
       </c>
       <c r="CH14" s="9"/>
-      <c r="CI14" s="49" t="s">
-        <v>214</v>
-      </c>
-      <c r="CJ14" s="49"/>
-      <c r="CK14" s="49"/>
-      <c r="DN14" s="49" t="s">
-        <v>215</v>
-      </c>
-      <c r="DO14" s="49"/>
+      <c r="CI14" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="CJ14" s="40"/>
+      <c r="CK14" s="40"/>
+      <c r="DN14" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="DO14" s="40"/>
       <c r="DP14" s="9"/>
       <c r="DQ14" s="9" t="s">
         <v>41</v>
       </c>
       <c r="DR14" s="9"/>
-      <c r="DS14" s="49" t="s">
-        <v>216</v>
-      </c>
-      <c r="DT14" s="49"/>
-      <c r="DU14" s="49"/>
+      <c r="DS14" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="DT14" s="40"/>
+      <c r="DU14" s="40"/>
     </row>
-    <row r="15" spans="1:125" ht="15" customHeight="1">
-      <c r="AK15" s="61" t="s">
-        <v>115</v>
-      </c>
-      <c r="AL15" s="61"/>
+    <row r="15" spans="1:125" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AK15" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL15" s="46"/>
       <c r="AM15" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="AN15" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="AO15" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AP15" s="61" t="s">
-        <v>119</v>
-      </c>
-      <c r="AQ15" s="61"/>
-      <c r="AR15" s="61"/>
-      <c r="AT15" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="AU15" s="49"/>
+        <v>109</v>
+      </c>
+      <c r="AP15" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="AQ15" s="46"/>
+      <c r="AR15" s="46"/>
+      <c r="AT15" s="40" t="s">
+        <v>204</v>
+      </c>
+      <c r="AU15" s="40"/>
       <c r="AV15" s="9"/>
       <c r="AW15" s="9" t="s">
         <v>41</v>
@@ -4618,43 +4624,43 @@
       <c r="AX15" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AY15" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="AZ15" s="56"/>
+      <c r="AY15" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="AZ15" s="70"/>
       <c r="BA15" s="57"/>
-      <c r="BU15" s="44" t="s">
-        <v>115</v>
+      <c r="BU15" s="43" t="s">
+        <v>106</v>
       </c>
       <c r="BV15" s="45"/>
       <c r="BW15" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="BX15" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="BY15" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="BZ15" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="CA15" s="26"/>
-      <c r="CB15" s="27"/>
-      <c r="CD15" s="77"/>
-      <c r="CE15" s="77"/>
-      <c r="CF15" s="78"/>
-      <c r="CG15" s="78"/>
-      <c r="CH15" s="78"/>
-      <c r="CI15" s="77"/>
-      <c r="CJ15" s="77"/>
-      <c r="CK15" s="77"/>
+        <v>109</v>
+      </c>
+      <c r="BZ15" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="CA15" s="44"/>
+      <c r="CB15" s="45"/>
+      <c r="CD15" s="41"/>
+      <c r="CE15" s="41"/>
+      <c r="CF15" s="39"/>
+      <c r="CG15" s="39"/>
+      <c r="CH15" s="39"/>
+      <c r="CI15" s="41"/>
+      <c r="CJ15" s="41"/>
+      <c r="CK15" s="41"/>
     </row>
-    <row r="16" spans="1:125" ht="15.75" customHeight="1">
-      <c r="AK16" s="69" t="s">
-        <v>218</v>
-      </c>
-      <c r="AL16" s="70"/>
+    <row r="16" spans="1:125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AK16" s="47" t="s">
+        <v>205</v>
+      </c>
+      <c r="AL16" s="48"/>
       <c r="AM16" s="4" t="s">
         <v>41</v>
       </c>
@@ -4662,90 +4668,251 @@
       <c r="AO16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AP16" s="69" t="s">
+      <c r="AP16" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="AQ16" s="71"/>
-      <c r="AR16" s="70"/>
-      <c r="BU16" s="42" t="s">
-        <v>219</v>
-      </c>
-      <c r="BV16" s="43"/>
-      <c r="BW16" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="BX16" s="40"/>
-      <c r="BY16" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="BZ16" s="37" t="s">
+      <c r="AQ16" s="49"/>
+      <c r="AR16" s="48"/>
+      <c r="BU16" s="53" t="s">
+        <v>206</v>
+      </c>
+      <c r="BV16" s="54"/>
+      <c r="BW16" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="BX16" s="37"/>
+      <c r="BY16" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="BZ16" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="CA16" s="41"/>
-      <c r="CB16" s="38"/>
+      <c r="CA16" s="38"/>
+      <c r="CB16" s="35"/>
     </row>
-    <row r="17" spans="73:80">
-      <c r="BU17" s="49" t="s">
-        <v>220</v>
-      </c>
-      <c r="BV17" s="49"/>
+    <row r="17" spans="73:80" x14ac:dyDescent="0.25">
+      <c r="BU17" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="BV17" s="40"/>
       <c r="BW17" s="9"/>
       <c r="BX17" s="9" t="s">
         <v>41</v>
       </c>
       <c r="BY17" s="9"/>
-      <c r="BZ17" s="49" t="s">
-        <v>221</v>
-      </c>
-      <c r="CA17" s="49"/>
-      <c r="CB17" s="49"/>
+      <c r="BZ17" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="CA17" s="40"/>
+      <c r="CB17" s="40"/>
     </row>
-    <row r="18" spans="73:80">
-      <c r="BU18" s="76" t="s">
-        <v>222</v>
-      </c>
-      <c r="BV18" s="76"/>
+    <row r="18" spans="73:80" x14ac:dyDescent="0.25">
+      <c r="BU18" s="75" t="s">
+        <v>209</v>
+      </c>
+      <c r="BV18" s="75"/>
       <c r="BW18" s="12"/>
       <c r="BX18" s="12" t="s">
         <v>41</v>
       </c>
       <c r="BY18" s="12"/>
-      <c r="BZ18" s="76" t="s">
-        <v>157</v>
-      </c>
-      <c r="CA18" s="76"/>
-      <c r="CB18" s="76"/>
+      <c r="BZ18" s="75" t="s">
+        <v>148</v>
+      </c>
+      <c r="CA18" s="75"/>
+      <c r="CB18" s="75"/>
     </row>
-    <row r="19" spans="73:80">
-      <c r="BU19" s="49" t="s">
-        <v>223</v>
-      </c>
-      <c r="BV19" s="49"/>
+    <row r="19" spans="73:80" x14ac:dyDescent="0.25">
+      <c r="BU19" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="BV19" s="40"/>
       <c r="BW19" s="9"/>
       <c r="BX19" s="9" t="s">
         <v>41</v>
       </c>
       <c r="BY19" s="9"/>
-      <c r="BZ19" s="49" t="s">
-        <v>224</v>
-      </c>
-      <c r="CA19" s="49"/>
-      <c r="CB19" s="49"/>
+      <c r="BZ19" s="40" t="s">
+        <v>211</v>
+      </c>
+      <c r="CA19" s="40"/>
+      <c r="CB19" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="213">
-    <mergeCell ref="BZ19:CB19"/>
-    <mergeCell ref="BU19:BV19"/>
-    <mergeCell ref="CD14:CE14"/>
-    <mergeCell ref="CI14:CK14"/>
-    <mergeCell ref="CD15:CE15"/>
-    <mergeCell ref="CI15:CK15"/>
-    <mergeCell ref="BL6:BM6"/>
-    <mergeCell ref="BL7:BS7"/>
-    <mergeCell ref="BL8:BM8"/>
-    <mergeCell ref="BQ8:BS8"/>
-    <mergeCell ref="BL9:BM9"/>
-    <mergeCell ref="BQ9:BS9"/>
+  <mergeCells count="216">
+    <mergeCell ref="DN14:DO14"/>
+    <mergeCell ref="DS13:DU13"/>
+    <mergeCell ref="DN13:DO13"/>
+    <mergeCell ref="DE10:DL10"/>
+    <mergeCell ref="CV10:DC10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="CD10:CE10"/>
+    <mergeCell ref="CD12:CE12"/>
+    <mergeCell ref="CI12:CK12"/>
+    <mergeCell ref="CD13:CE13"/>
+    <mergeCell ref="BH11:BJ11"/>
+    <mergeCell ref="AT14:AU14"/>
+    <mergeCell ref="AY14:BA14"/>
+    <mergeCell ref="BC10:BD10"/>
+    <mergeCell ref="BC11:BD11"/>
+    <mergeCell ref="AK14:AR14"/>
+    <mergeCell ref="BU14:CB14"/>
+    <mergeCell ref="DE13:DF13"/>
+    <mergeCell ref="DJ13:DL13"/>
+    <mergeCell ref="CR10:CT10"/>
+    <mergeCell ref="DS12:DU12"/>
+    <mergeCell ref="AT15:AU15"/>
+    <mergeCell ref="AT12:BA12"/>
+    <mergeCell ref="AY15:BA15"/>
+    <mergeCell ref="BH10:BJ10"/>
+    <mergeCell ref="DN11:DU11"/>
+    <mergeCell ref="DS14:DU14"/>
+    <mergeCell ref="DE11:DF11"/>
+    <mergeCell ref="DJ11:DL11"/>
+    <mergeCell ref="DE12:DF12"/>
+    <mergeCell ref="DJ12:DL12"/>
+    <mergeCell ref="DN10:DO10"/>
+    <mergeCell ref="DN12:DO12"/>
+    <mergeCell ref="CM10:CN10"/>
+    <mergeCell ref="CM12:CN12"/>
+    <mergeCell ref="CR12:CT12"/>
+    <mergeCell ref="CM11:CN11"/>
+    <mergeCell ref="CV11:CW11"/>
+    <mergeCell ref="DA11:DC11"/>
+    <mergeCell ref="CV12:CW12"/>
+    <mergeCell ref="DA12:DC12"/>
+    <mergeCell ref="BU10:BV10"/>
+    <mergeCell ref="BU11:BV11"/>
+    <mergeCell ref="BU13:BV13"/>
+    <mergeCell ref="BU12:BV12"/>
+    <mergeCell ref="DO1:DU1"/>
+    <mergeCell ref="DO2:DU2"/>
+    <mergeCell ref="DN3:DU3"/>
+    <mergeCell ref="DN4:DO4"/>
+    <mergeCell ref="DN5:DO5"/>
+    <mergeCell ref="DN6:DO6"/>
+    <mergeCell ref="DN7:DO7"/>
+    <mergeCell ref="DN8:DO8"/>
+    <mergeCell ref="DN9:DO9"/>
+    <mergeCell ref="DF1:DL1"/>
+    <mergeCell ref="DF2:DL2"/>
+    <mergeCell ref="DE3:DL3"/>
+    <mergeCell ref="DE4:DF4"/>
+    <mergeCell ref="DE5:DF5"/>
+    <mergeCell ref="DE6:DF6"/>
+    <mergeCell ref="DE7:DF7"/>
+    <mergeCell ref="DE8:DF8"/>
+    <mergeCell ref="DE9:DF9"/>
+    <mergeCell ref="CM9:CT9"/>
+    <mergeCell ref="CW1:DC1"/>
+    <mergeCell ref="CW2:DC2"/>
+    <mergeCell ref="CV3:DC3"/>
+    <mergeCell ref="CV4:CW4"/>
+    <mergeCell ref="CV5:CW5"/>
+    <mergeCell ref="CV6:CW6"/>
+    <mergeCell ref="CV7:CW7"/>
+    <mergeCell ref="CV8:CW8"/>
+    <mergeCell ref="CV9:CW9"/>
+    <mergeCell ref="CN1:CT1"/>
+    <mergeCell ref="CN2:CT2"/>
+    <mergeCell ref="CM3:CT3"/>
+    <mergeCell ref="CM4:CN4"/>
+    <mergeCell ref="CM5:CN5"/>
+    <mergeCell ref="CM6:CN6"/>
+    <mergeCell ref="CM7:CN7"/>
+    <mergeCell ref="CM8:CN8"/>
+    <mergeCell ref="CE1:CK1"/>
+    <mergeCell ref="CE2:CK2"/>
+    <mergeCell ref="CD3:CK3"/>
+    <mergeCell ref="CD4:CE4"/>
+    <mergeCell ref="CD5:CE5"/>
+    <mergeCell ref="CD6:CE6"/>
+    <mergeCell ref="CD7:CE7"/>
+    <mergeCell ref="CD8:CE8"/>
+    <mergeCell ref="CD9:CE9"/>
+    <mergeCell ref="BV1:CB1"/>
+    <mergeCell ref="BV2:CB2"/>
+    <mergeCell ref="BU3:CB3"/>
+    <mergeCell ref="BU4:BV4"/>
+    <mergeCell ref="BU5:BV5"/>
+    <mergeCell ref="BU6:BV6"/>
+    <mergeCell ref="BU7:BV7"/>
+    <mergeCell ref="BU8:BV8"/>
+    <mergeCell ref="BU9:BV9"/>
+    <mergeCell ref="BD1:BJ1"/>
+    <mergeCell ref="BD2:BJ2"/>
+    <mergeCell ref="BC3:BJ3"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="BC7:BD7"/>
+    <mergeCell ref="BC8:BD8"/>
+    <mergeCell ref="BC9:BD9"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="AU2:BA2"/>
+    <mergeCell ref="AT3:BA3"/>
+    <mergeCell ref="AT4:AU4"/>
+    <mergeCell ref="AT5:AU5"/>
+    <mergeCell ref="AT11:AU11"/>
+    <mergeCell ref="AT13:AU13"/>
+    <mergeCell ref="AY13:BA13"/>
+    <mergeCell ref="AT6:AU6"/>
+    <mergeCell ref="AT7:AU7"/>
+    <mergeCell ref="AT8:AU8"/>
+    <mergeCell ref="AT9:AU9"/>
+    <mergeCell ref="AT10:AU10"/>
+    <mergeCell ref="AK15:AL15"/>
+    <mergeCell ref="AP15:AR15"/>
+    <mergeCell ref="AK16:AL16"/>
+    <mergeCell ref="AP16:AR16"/>
+    <mergeCell ref="AK10:AL10"/>
+    <mergeCell ref="AK11:AL11"/>
+    <mergeCell ref="AK12:AL12"/>
+    <mergeCell ref="AK13:AL13"/>
+    <mergeCell ref="AL1:AR1"/>
+    <mergeCell ref="AL2:AR2"/>
+    <mergeCell ref="AK3:AR3"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="AK7:AL7"/>
+    <mergeCell ref="AK8:AL8"/>
+    <mergeCell ref="AK9:AL9"/>
+    <mergeCell ref="X9:Z9"/>
+    <mergeCell ref="AC1:AI1"/>
+    <mergeCell ref="AC2:AI2"/>
+    <mergeCell ref="AB3:AI3"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AB9:AC9"/>
+    <mergeCell ref="AG12:AI12"/>
+    <mergeCell ref="AB12:AC12"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AB10:AI10"/>
+    <mergeCell ref="AB11:AC11"/>
+    <mergeCell ref="AG11:AI11"/>
+    <mergeCell ref="AB7:AC7"/>
+    <mergeCell ref="AB8:AC8"/>
+    <mergeCell ref="T1:Z1"/>
+    <mergeCell ref="T2:Z2"/>
+    <mergeCell ref="S3:Z3"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S7:Z7"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="J7:Q7"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="K1:Q1"/>
+    <mergeCell ref="K2:Q2"/>
+    <mergeCell ref="J3:Q3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="S9:T9"/>
     <mergeCell ref="BM1:BS1"/>
     <mergeCell ref="BM2:BS2"/>
     <mergeCell ref="BL3:BS3"/>
@@ -4770,183 +4937,25 @@
     <mergeCell ref="O8:Q8"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="O9:Q9"/>
-    <mergeCell ref="J7:Q7"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="K1:Q1"/>
-    <mergeCell ref="K2:Q2"/>
-    <mergeCell ref="J3:Q3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="X9:Z9"/>
-    <mergeCell ref="AC1:AI1"/>
-    <mergeCell ref="AC2:AI2"/>
-    <mergeCell ref="AB3:AI3"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AB9:AC9"/>
-    <mergeCell ref="AG12:AI12"/>
-    <mergeCell ref="AB12:AC12"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AB10:AI10"/>
-    <mergeCell ref="AB11:AC11"/>
-    <mergeCell ref="AG11:AI11"/>
-    <mergeCell ref="AB7:AC7"/>
-    <mergeCell ref="AB8:AC8"/>
-    <mergeCell ref="T1:Z1"/>
-    <mergeCell ref="T2:Z2"/>
-    <mergeCell ref="S3:Z3"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="S7:Z7"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="AK15:AL15"/>
-    <mergeCell ref="AP15:AR15"/>
-    <mergeCell ref="AK16:AL16"/>
-    <mergeCell ref="AP16:AR16"/>
-    <mergeCell ref="AK10:AL10"/>
-    <mergeCell ref="AK11:AL11"/>
-    <mergeCell ref="AK12:AL12"/>
-    <mergeCell ref="AK13:AL13"/>
-    <mergeCell ref="AL1:AR1"/>
-    <mergeCell ref="AL2:AR2"/>
-    <mergeCell ref="AK3:AR3"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="AK7:AL7"/>
-    <mergeCell ref="AK8:AL8"/>
-    <mergeCell ref="AK9:AL9"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="AU2:BA2"/>
-    <mergeCell ref="AT3:BA3"/>
-    <mergeCell ref="AT4:AU4"/>
-    <mergeCell ref="AT5:AU5"/>
-    <mergeCell ref="AT11:AU11"/>
-    <mergeCell ref="AT13:AU13"/>
-    <mergeCell ref="AY13:BA13"/>
-    <mergeCell ref="AT6:AU6"/>
-    <mergeCell ref="AT7:AU7"/>
-    <mergeCell ref="AT8:AU8"/>
-    <mergeCell ref="AT9:AU9"/>
-    <mergeCell ref="AT10:AU10"/>
-    <mergeCell ref="BD1:BJ1"/>
-    <mergeCell ref="BD2:BJ2"/>
-    <mergeCell ref="BC3:BJ3"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="BC7:BD7"/>
-    <mergeCell ref="BC8:BD8"/>
-    <mergeCell ref="BC9:BD9"/>
-    <mergeCell ref="BV1:CB1"/>
-    <mergeCell ref="BV2:CB2"/>
-    <mergeCell ref="BU3:CB3"/>
-    <mergeCell ref="BU4:BV4"/>
-    <mergeCell ref="BU5:BV5"/>
-    <mergeCell ref="BU6:BV6"/>
-    <mergeCell ref="BU7:BV7"/>
-    <mergeCell ref="BU8:BV8"/>
-    <mergeCell ref="BU9:BV9"/>
-    <mergeCell ref="CE1:CK1"/>
-    <mergeCell ref="CE2:CK2"/>
-    <mergeCell ref="CD3:CK3"/>
-    <mergeCell ref="CD4:CE4"/>
-    <mergeCell ref="CD5:CE5"/>
-    <mergeCell ref="CD6:CE6"/>
-    <mergeCell ref="CD7:CE7"/>
-    <mergeCell ref="CD8:CE8"/>
-    <mergeCell ref="CD9:CE9"/>
-    <mergeCell ref="CM9:CT9"/>
-    <mergeCell ref="CW1:DC1"/>
-    <mergeCell ref="CW2:DC2"/>
-    <mergeCell ref="CV3:DC3"/>
-    <mergeCell ref="CV4:CW4"/>
-    <mergeCell ref="CV5:CW5"/>
-    <mergeCell ref="CV6:CW6"/>
-    <mergeCell ref="CV7:CW7"/>
-    <mergeCell ref="CV8:CW8"/>
-    <mergeCell ref="CV9:CW9"/>
-    <mergeCell ref="CN1:CT1"/>
-    <mergeCell ref="CN2:CT2"/>
-    <mergeCell ref="CM3:CT3"/>
-    <mergeCell ref="CM4:CN4"/>
-    <mergeCell ref="CM5:CN5"/>
-    <mergeCell ref="CM6:CN6"/>
-    <mergeCell ref="CM7:CN7"/>
-    <mergeCell ref="CM8:CN8"/>
-    <mergeCell ref="DF1:DL1"/>
-    <mergeCell ref="DF2:DL2"/>
-    <mergeCell ref="DE3:DL3"/>
-    <mergeCell ref="DE4:DF4"/>
-    <mergeCell ref="DE5:DF5"/>
-    <mergeCell ref="DE6:DF6"/>
-    <mergeCell ref="DE7:DF7"/>
-    <mergeCell ref="DE8:DF8"/>
-    <mergeCell ref="DE9:DF9"/>
-    <mergeCell ref="DO1:DU1"/>
-    <mergeCell ref="DO2:DU2"/>
-    <mergeCell ref="DN3:DU3"/>
-    <mergeCell ref="DN4:DO4"/>
-    <mergeCell ref="DN5:DO5"/>
-    <mergeCell ref="DN6:DO6"/>
-    <mergeCell ref="DN7:DO7"/>
-    <mergeCell ref="DN8:DO8"/>
-    <mergeCell ref="DN9:DO9"/>
-    <mergeCell ref="AT15:AU15"/>
-    <mergeCell ref="AT12:BA12"/>
-    <mergeCell ref="AY15:BA15"/>
-    <mergeCell ref="BH10:BJ10"/>
-    <mergeCell ref="DN11:DU11"/>
-    <mergeCell ref="DS14:DU14"/>
-    <mergeCell ref="DE11:DF11"/>
-    <mergeCell ref="DJ11:DL11"/>
-    <mergeCell ref="DE12:DF12"/>
-    <mergeCell ref="DJ12:DL12"/>
-    <mergeCell ref="DN10:DO10"/>
-    <mergeCell ref="DN12:DO12"/>
-    <mergeCell ref="CM10:CN10"/>
-    <mergeCell ref="CM12:CN12"/>
-    <mergeCell ref="CR12:CT12"/>
-    <mergeCell ref="CM11:CN11"/>
-    <mergeCell ref="CV11:CW11"/>
-    <mergeCell ref="DA11:DC11"/>
-    <mergeCell ref="CV12:CW12"/>
-    <mergeCell ref="DA12:DC12"/>
-    <mergeCell ref="BU10:BV10"/>
-    <mergeCell ref="BU11:BV11"/>
-    <mergeCell ref="BU13:BV13"/>
-    <mergeCell ref="BU12:BV12"/>
-    <mergeCell ref="DN14:DO14"/>
-    <mergeCell ref="DS13:DU13"/>
-    <mergeCell ref="DN13:DO13"/>
-    <mergeCell ref="DE10:DL10"/>
-    <mergeCell ref="CV10:DC10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="CD10:CE10"/>
-    <mergeCell ref="CD12:CE12"/>
-    <mergeCell ref="CI12:CK12"/>
-    <mergeCell ref="CD13:CE13"/>
-    <mergeCell ref="BH11:BJ11"/>
-    <mergeCell ref="AT14:AU14"/>
-    <mergeCell ref="AY14:BA14"/>
-    <mergeCell ref="BC10:BD10"/>
-    <mergeCell ref="BC11:BD11"/>
-    <mergeCell ref="AK14:AR14"/>
+    <mergeCell ref="BZ19:CB19"/>
+    <mergeCell ref="BU19:BV19"/>
+    <mergeCell ref="CD14:CE14"/>
+    <mergeCell ref="CI14:CK14"/>
+    <mergeCell ref="CD15:CE15"/>
+    <mergeCell ref="CI15:CK15"/>
+    <mergeCell ref="BL6:BM6"/>
+    <mergeCell ref="BL7:BS7"/>
+    <mergeCell ref="BL8:BM8"/>
+    <mergeCell ref="BQ8:BS8"/>
+    <mergeCell ref="BL9:BM9"/>
+    <mergeCell ref="BQ9:BS9"/>
     <mergeCell ref="BU16:BV16"/>
     <mergeCell ref="BU15:BV15"/>
-    <mergeCell ref="BU14:CB14"/>
     <mergeCell ref="BU17:BV17"/>
     <mergeCell ref="BU18:BV18"/>
     <mergeCell ref="BZ17:CB17"/>
     <mergeCell ref="BZ18:CB18"/>
-    <mergeCell ref="DE13:DF13"/>
-    <mergeCell ref="DJ13:DL13"/>
+    <mergeCell ref="BZ15:CB15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>